<commit_message>
Add 14 Atlas AI cards for openEuler 20.03LTS/22.03LTS
</commit_message>
<xml_diff>
--- a/data/compatibility/openEuler20.03-LTS上两类平台板卡兼容清单.xlsx
+++ b/data/compatibility/openEuler20.03-LTS上两类平台板卡兼容清单.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20389"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work Station\Gitee\openEuler-portal\data\compatibility\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC5DAF67-C9B9-420F-9BB7-F1959F6E9EFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="11940" tabRatio="603"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28130" windowHeight="11940" tabRatio="603" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="openEuler20.03-LTS-SP1两类平台板卡兼容性" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="274">
   <si>
     <t>vendorID</t>
   </si>
@@ -918,18 +924,88 @@
   <si>
     <t>RU150-M</t>
   </si>
+  <si>
+    <t>19e5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>d100</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0200</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0100</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>npu</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022.09.21</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Huawei</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Atlas 300I(Model 3010)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://support.huawei.com/enterprise/zh/ascend-computing/a300-3010-pid-251560253/software</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>d500</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Atlas 300I(Model 9000)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Atlas 300I Pro</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Atlas 300V Pro</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>AI</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>02313FUJ</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>02313SHF/02314BCJ</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://support.huawei.com/enterprise/zh/ascend-computing/a300t-9000-pid-250702906/software</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://support.huawei.com/enterprise/zh/ascend-computing/atlas-300i-pro-pid-251052354/software</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>d801</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -958,143 +1034,28 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="9"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="37">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1109,7 +1070,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.0499893185216834"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1125,194 +1086,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1335,249 +1110,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1585,15 +1121,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="50">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="49">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="49" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1653,67 +1189,28 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="10" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="10" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="4">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
-    <cellStyle name="常规 2" xfId="49"/>
-    <cellStyle name="常规 3" xfId="50"/>
+    <cellStyle name="常规 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="常规 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2000,43 +1497,42 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:R54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="F61" sqref="F61"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="10.625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="8.75" style="9" customWidth="1"/>
-    <col min="4" max="4" width="10.5" style="9" customWidth="1"/>
-    <col min="5" max="5" width="10.25" style="9" customWidth="1"/>
-    <col min="6" max="6" width="27.5" style="9" customWidth="1"/>
-    <col min="7" max="7" width="15.25" style="9" customWidth="1"/>
-    <col min="8" max="8" width="24.875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="11.08984375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="27.453125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="15.26953125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="24.90625" style="9" customWidth="1"/>
     <col min="9" max="9" width="11" style="9" customWidth="1"/>
-    <col min="10" max="10" width="13.125" style="9" customWidth="1"/>
+    <col min="10" max="10" width="13.08984375" style="9" customWidth="1"/>
     <col min="11" max="11" width="65" style="9" customWidth="1"/>
-    <col min="12" max="12" width="16.625" style="9" customWidth="1"/>
-    <col min="13" max="13" width="17.375" style="9" customWidth="1"/>
-    <col min="14" max="14" width="32.75" style="9" customWidth="1"/>
+    <col min="12" max="12" width="16.6328125" style="9" customWidth="1"/>
+    <col min="13" max="13" width="17.36328125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="32.7265625" style="9" customWidth="1"/>
     <col min="15" max="15" width="42" style="9" customWidth="1"/>
-    <col min="16" max="16" width="22.25" style="10" customWidth="1"/>
+    <col min="16" max="16" width="22.26953125" style="10" customWidth="1"/>
     <col min="17" max="17" width="189" style="9" customWidth="1"/>
     <col min="18" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="1" ht="20.25" customHeight="1" spans="1:18">
+    <row r="1" spans="1:18" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -2092,7 +1588,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" s="5" customFormat="1" spans="1:17">
+    <row r="2" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
@@ -2145,7 +1641,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>19</v>
       </c>
@@ -2195,7 +1691,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>19</v>
       </c>
@@ -2245,7 +1741,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>19</v>
       </c>
@@ -2295,7 +1791,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>19</v>
       </c>
@@ -2345,7 +1841,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>19</v>
       </c>
@@ -2395,7 +1891,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>52</v>
       </c>
@@ -2448,7 +1944,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" s="6" customFormat="1" spans="1:17">
+    <row r="9" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>52</v>
       </c>
@@ -2501,7 +1997,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>68</v>
       </c>
@@ -2549,7 +2045,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>68</v>
       </c>
@@ -2599,7 +2095,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>68</v>
       </c>
@@ -2649,7 +2145,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>68</v>
       </c>
@@ -2700,7 +2196,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>68</v>
       </c>
@@ -2751,7 +2247,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>68</v>
       </c>
@@ -2802,7 +2298,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>101</v>
       </c>
@@ -2853,7 +2349,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>52</v>
       </c>
@@ -2904,7 +2400,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>52</v>
       </c>
@@ -2953,7 +2449,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>52</v>
       </c>
@@ -3002,7 +2498,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>52</v>
       </c>
@@ -3051,7 +2547,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>68</v>
       </c>
@@ -3102,7 +2598,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>68</v>
       </c>
@@ -3153,7 +2649,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>68</v>
       </c>
@@ -3204,7 +2700,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>68</v>
       </c>
@@ -3255,7 +2751,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>68</v>
       </c>
@@ -3306,7 +2802,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
         <v>154</v>
       </c>
@@ -3357,7 +2853,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="18">
         <v>8086</v>
       </c>
@@ -3408,7 +2904,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="18">
         <v>8086</v>
       </c>
@@ -3459,7 +2955,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="18">
         <v>8086</v>
       </c>
@@ -3510,7 +3006,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" s="6" customFormat="1" spans="1:17">
+    <row r="30" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="19">
         <v>8086</v>
       </c>
@@ -3561,7 +3057,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="31" s="6" customFormat="1" spans="1:17">
+    <row r="31" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19">
         <v>8086</v>
       </c>
@@ -3612,7 +3108,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="32" s="6" customFormat="1" spans="1:17">
+    <row r="32" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="19">
         <v>8086</v>
       </c>
@@ -3663,7 +3159,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="18">
         <v>8086</v>
       </c>
@@ -3714,7 +3210,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="18">
         <v>1000</v>
       </c>
@@ -3765,7 +3261,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="35" spans="1:17">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="18">
         <v>1000</v>
       </c>
@@ -3816,7 +3312,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="18">
         <v>1000</v>
       </c>
@@ -3867,7 +3363,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="18">
         <v>1000</v>
       </c>
@@ -3918,7 +3414,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="18">
         <v>1000</v>
       </c>
@@ -3969,7 +3465,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="18">
         <v>1000</v>
       </c>
@@ -4020,7 +3516,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="40" spans="1:17">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="18">
         <v>1000</v>
       </c>
@@ -4071,7 +3567,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="18">
         <v>1000</v>
       </c>
@@ -4122,7 +3618,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="42" s="7" customFormat="1" spans="1:17">
+    <row r="42" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="21">
         <v>1000</v>
       </c>
@@ -4173,7 +3669,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>222</v>
       </c>
@@ -4221,7 +3717,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="44" s="8" customFormat="1" ht="14.45" customHeight="1" spans="1:17">
+    <row r="44" spans="1:17" s="8" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
         <v>222</v>
       </c>
@@ -4270,7 +3766,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>222</v>
       </c>
@@ -4317,7 +3813,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="46" spans="1:17">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>222</v>
       </c>
@@ -4364,7 +3860,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="47" spans="1:17">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="18">
         <v>1000</v>
       </c>
@@ -4413,7 +3909,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="48" spans="1:17">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="18">
         <v>1000</v>
       </c>
@@ -4462,7 +3958,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="49" spans="1:17">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="18">
         <v>1000</v>
       </c>
@@ -4511,7 +4007,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="50" spans="1:17">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="18">
         <v>1000</v>
       </c>
@@ -4560,7 +4056,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="51" spans="1:17">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="18">
         <v>1000</v>
       </c>
@@ -4609,7 +4105,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="52" spans="1:17">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>101</v>
       </c>
@@ -4659,7 +4155,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="53" spans="1:17">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>101</v>
       </c>
@@ -4707,7 +4203,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="54" spans="1:17">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>101</v>
       </c>
@@ -4755,74 +4251,420 @@
         <v>252</v>
       </c>
     </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A55" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="B55" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="C55" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="D55" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G55" s="32" t="s">
+        <v>259</v>
+      </c>
+      <c r="I55" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="J55" s="32" t="s">
+        <v>260</v>
+      </c>
+      <c r="M55" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="N55" s="32" t="s">
+        <v>262</v>
+      </c>
+      <c r="O55" s="32" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q55" s="29" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A56" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="B56" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="C56" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="D56" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="E56" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G56" s="32" t="s">
+        <v>259</v>
+      </c>
+      <c r="I56" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="J56" s="32" t="s">
+        <v>260</v>
+      </c>
+      <c r="M56" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="N56" s="32" t="s">
+        <v>262</v>
+      </c>
+      <c r="O56" s="32" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q56" s="29" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A57" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="B57" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="C57" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="D57" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G57" s="32" t="s">
+        <v>259</v>
+      </c>
+      <c r="I57" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="J57" s="32" t="s">
+        <v>260</v>
+      </c>
+      <c r="M57" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="N57" s="32" t="s">
+        <v>265</v>
+      </c>
+      <c r="O57" s="32" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q57" s="29" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A58" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="B58" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="C58" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="D58" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="E58" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="F58" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G58" s="32" t="s">
+        <v>259</v>
+      </c>
+      <c r="I58" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="J58" s="32" t="s">
+        <v>260</v>
+      </c>
+      <c r="M58" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="N58" s="32" t="s">
+        <v>265</v>
+      </c>
+      <c r="O58" s="32" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q58" s="29" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A59" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="B59" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="C59" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="D59" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G59" s="32" t="s">
+        <v>259</v>
+      </c>
+      <c r="I59" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="J59" s="32" t="s">
+        <v>260</v>
+      </c>
+      <c r="M59" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="N59" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="O59" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="P59" s="33" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q59" s="29" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A60" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="B60" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="C60" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="D60" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="E60" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G60" s="32" t="s">
+        <v>259</v>
+      </c>
+      <c r="I60" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="J60" s="32" t="s">
+        <v>260</v>
+      </c>
+      <c r="M60" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="N60" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="O60" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="P60" s="33" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q60" s="29" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A61" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="B61" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="C61" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="D61" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G61" s="32" t="s">
+        <v>259</v>
+      </c>
+      <c r="I61" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="J61" s="32" t="s">
+        <v>260</v>
+      </c>
+      <c r="M61" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="N61" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="O61" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="P61" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q61" s="29" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A62" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="B62" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="C62" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="D62" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="E62" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="F62" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G62" s="32" t="s">
+        <v>259</v>
+      </c>
+      <c r="I62" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="J62" s="32" t="s">
+        <v>260</v>
+      </c>
+      <c r="M62" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="N62" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="O62" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="P62" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q62" s="29" t="s">
+        <v>272</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:Q52">
-    <extLst/>
-  </autoFilter>
+  <autoFilter ref="A1:Q52" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="Q10" r:id="rId1" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/source/Packages/MLNX_OFED_LINUX-5.1-2.5.2.0-openeuler20.03-aarch64-ext.tgz"/>
-    <hyperlink ref="Q3" r:id="rId2" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/noarch/Packages/qla2xxx-10.02.04.00_k-1dkms.noarch.rpm"/>
-    <hyperlink ref="Q19" r:id="rId3" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/aarch64/Packages/NIC-IN200-openEuler20.03-hinic-3.7.0.8-aarch64.rpm"/>
-    <hyperlink ref="Q20" r:id="rId4" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/aarch64/Packages/NIC-IN200-openEuler20.03-hinic-3.7.0.8-aarch64.rpm"/>
-    <hyperlink ref="Q35" r:id="rId5" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/x86_64/Packages/RAID-3004iMR_3108_3408iMR_3416iMR_3508_3516-openEuler20.03-megaraid_sas-07.714.04.00-1-x86_64.rpm"/>
-    <hyperlink ref="Q4:Q7" r:id="rId2" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/noarch/Packages/qla2xxx-10.02.04.00_k-1dkms.noarch.rpm"/>
-    <hyperlink ref="Q11:Q12" r:id="rId1" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/source/Packages/MLNX_OFED_LINUX-5.1-2.5.2.0-openeuler20.03-aarch64-ext.tgz"/>
-    <hyperlink ref="Q13:Q15" r:id="rId1" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/source/Packages/MLNX_OFED_LINUX-5.1-2.5.2.0-openeuler20.03-aarch64-ext.tgz"/>
-    <hyperlink ref="Q34" r:id="rId5" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/x86_64/Packages/RAID-3004iMR_3108_3408iMR_3416iMR_3508_3516-openEuler20.03-megaraid_sas-07.714.04.00-1-x86_64.rpm"/>
-    <hyperlink ref="Q36" r:id="rId5" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/x86_64/Packages/RAID-3004iMR_3108_3408iMR_3416iMR_3508_3516-openEuler20.03-megaraid_sas-07.714.04.00-1-x86_64.rpm"/>
-    <hyperlink ref="Q37" r:id="rId5" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/x86_64/Packages/RAID-3004iMR_3108_3408iMR_3416iMR_3508_3516-openEuler20.03-megaraid_sas-07.714.04.00-1-x86_64.rpm"/>
-    <hyperlink ref="Q38" r:id="rId5" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/x86_64/Packages/RAID-3004iMR_3108_3408iMR_3416iMR_3508_3516-openEuler20.03-megaraid_sas-07.714.04.00-1-x86_64.rpm"/>
-    <hyperlink ref="Q39" r:id="rId5" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/x86_64/Packages/RAID-3004iMR_3108_3408iMR_3416iMR_3508_3516-openEuler20.03-megaraid_sas-07.714.04.00-1-x86_64.rpm"/>
-    <hyperlink ref="Q40" r:id="rId5" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/x86_64/Packages/RAID-3004iMR_3108_3408iMR_3416iMR_3508_3516-openEuler20.03-megaraid_sas-07.714.04.00-1-x86_64.rpm"/>
-    <hyperlink ref="Q41" r:id="rId5" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/x86_64/Packages/RAID-3004iMR_3108_3408iMR_3416iMR_3508_3516-openEuler20.03-megaraid_sas-07.714.04.00-1-x86_64.rpm"/>
-    <hyperlink ref="Q16" r:id="rId6" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/aarch64/Packages/RAID-3408iMR_3416iMR_3508_3516-openEuler20.03-megaraid_sas-07.714.04.00-aarch64.rpm"/>
-    <hyperlink ref="Q28" r:id="rId7" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/x86_64/Packages/NIC-X710_X722_XL710_XXV710-openEuler20.03SP1-i40e-2.12.6-1-x86_64.rpm"/>
-    <hyperlink ref="Q17" r:id="rId8" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/aarch64/Packages/FC-IN300-openEuler20.03-hifc-3.7.0.8-aarch64.rpm"/>
-    <hyperlink ref="Q43" r:id="rId9" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/source/Packages/elx_elx-lpfc-dd-openEuler20-12.8.542.29-ds-1.tar.gz"/>
-    <hyperlink ref="Q47" r:id="rId5" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/x86_64/Packages/RAID-3004iMR_3108_3408iMR_3416iMR_3508_3516-openEuler20.03-megaraid_sas-07.714.04.00-1-x86_64.rpm"/>
-    <hyperlink ref="Q48" r:id="rId5" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/x86_64/Packages/RAID-3004iMR_3108_3408iMR_3416iMR_3508_3516-openEuler20.03-megaraid_sas-07.714.04.00-1-x86_64.rpm"/>
-    <hyperlink ref="Q49" r:id="rId5" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/x86_64/Packages/RAID-3004iMR_3108_3408iMR_3416iMR_3508_3516-openEuler20.03-megaraid_sas-07.714.04.00-1-x86_64.rpm"/>
-    <hyperlink ref="Q50" r:id="rId5" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/x86_64/Packages/RAID-3004iMR_3108_3408iMR_3416iMR_3508_3516-openEuler20.03-megaraid_sas-07.714.04.00-1-x86_64.rpm"/>
-    <hyperlink ref="Q51" r:id="rId5" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/x86_64/Packages/RAID-3004iMR_3108_3408iMR_3416iMR_3508_3516-openEuler20.03-megaraid_sas-07.714.04.00-1-x86_64.rpm"/>
-    <hyperlink ref="Q52" r:id="rId10" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/source/Packages/MR_LINUX_DRIVER_7.22-07.722.02.00-2.tgz"/>
-    <hyperlink ref="Q53" r:id="rId10" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/source/Packages/MR_LINUX_DRIVER_7.22-07.722.02.00-2.tgz"/>
-    <hyperlink ref="Q54" r:id="rId10" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/source/Packages/MR_LINUX_DRIVER_7.22-07.722.02.00-2.tgz"/>
+    <hyperlink ref="Q10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="Q3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="Q19" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="Q20" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="Q35" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="Q4:Q7" r:id="rId6" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/noarch/Packages/qla2xxx-10.02.04.00_k-1dkms.noarch.rpm" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="Q11:Q12" r:id="rId7" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/source/Packages/MLNX_OFED_LINUX-5.1-2.5.2.0-openeuler20.03-aarch64-ext.tgz" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="Q13:Q15" r:id="rId8" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS/contrib/drivers/source/Packages/MLNX_OFED_LINUX-5.1-2.5.2.0-openeuler20.03-aarch64-ext.tgz" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="Q34" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="Q36" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="Q37" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="Q38" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="Q39" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="Q40" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="Q41" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="Q16" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="Q28" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="Q17" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="Q43" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="Q47" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="Q48" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="Q49" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="Q50" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="Q51" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="Q52" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="Q53" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="Q54" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="Q55" r:id="rId28" xr:uid="{471E354B-126D-423E-98D7-A60DF9817ECF}"/>
+    <hyperlink ref="Q57" r:id="rId29" xr:uid="{6E3A89D6-CF0D-41F1-9BE4-4E23FA2CD5C9}"/>
+    <hyperlink ref="Q59" r:id="rId30" xr:uid="{6981D348-DA98-4F8C-BE68-1989932B3096}"/>
+    <hyperlink ref="Q60" r:id="rId31" xr:uid="{DBCA1C85-B6A4-43C6-A25F-B6D82F919B06}"/>
+    <hyperlink ref="Q61" r:id="rId32" xr:uid="{30ED7BB5-B69C-470A-AC33-8962AD068294}"/>
+    <hyperlink ref="Q58" r:id="rId33" xr:uid="{805F6679-442C-436D-9DA5-2FAC4EE45BA5}"/>
+    <hyperlink ref="Q56" r:id="rId34" xr:uid="{3608A943-6A79-4468-BF97-A081D1A321E2}"/>
+    <hyperlink ref="Q62" r:id="rId35" xr:uid="{7D249D7F-CCD6-43AB-91C6-A1DD910827CD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180"/>
-  <headerFooter/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId36"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21.125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.5" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.6328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21.08984375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" style="2" customWidth="1"/>
     <col min="4" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.748031496062992" right="0.748031496062992" top="0.984251968503937" bottom="0.984251968503937" header="0.511811023622047" footer="0.511811023622047"/>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.74803149606299202" right="0.74803149606299202" top="0.98425196850393704" bottom="0.98425196850393704" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;G&amp;C&amp;F&amp;R文档密级</oddHeader>
@@ -4833,20 +4675,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData/>
-  <pageMargins left="0.748031496062992" right="0.748031496062992" top="0.984251968503937" bottom="0.984251968503937" header="0.511811023622047" footer="0.511811023622047"/>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.74803149606299202" right="0.74803149606299202" top="0.98425196850393704" bottom="0.98425196850393704" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;G&amp;C&amp;F&amp;R文档密级</oddHeader>

</xml_diff>

<commit_message>
update sha256 and driversize for inbox driver
</commit_message>
<xml_diff>
--- a/data/compatibility/openEuler20.03-LTS上两类平台板卡兼容清单.xlsx
+++ b/data/compatibility/openEuler20.03-LTS上两类平台板卡兼容清单.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="288">
   <si>
     <t>vendorID</t>
   </si>
@@ -108,7 +108,7 @@
     <t>9659e6a4efe55eb5eb93187f131c670bae71099f819f66660c249467c2920eed</t>
   </si>
   <si>
-    <t>1.1M</t>
+    <t>1.1MB</t>
   </si>
   <si>
     <t>Marvell/Qlogic</t>
@@ -201,10 +201,10 @@
     <t>2020.05.07</t>
   </si>
   <si>
-    <t>4C5D1B8BFF927AAADF5D6AFC162F91CE0445A417</t>
-  </si>
-  <si>
-    <t>164KB</t>
+    <t>7f4468b8ddafd4c342807c5aef89331b1aae42bff1c435900f616d2248d6f6d3</t>
+  </si>
+  <si>
+    <t>163KB</t>
   </si>
   <si>
     <t>Huawei</t>
@@ -225,28 +225,6 @@
     <t>a221</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>164K</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>B</t>
-    </r>
-  </si>
-  <si>
     <t>15b3</t>
   </si>
   <si>
@@ -268,7 +246,7 @@
     <t>4fe122539579e01fda71769c1fb0b8782df6368a1a6f68e2cf78d0a7a4879b74</t>
   </si>
   <si>
-    <t>242M</t>
+    <t>242MB</t>
   </si>
   <si>
     <t>Mellanox</t>
@@ -463,7 +441,7 @@
     <t>ddaa6657252f691c8121ba8ad61ab7339ac559c3efa4fe90e33bec40c3269543</t>
   </si>
   <si>
-    <t xml:space="preserve">273K </t>
+    <t>273KB</t>
   </si>
   <si>
     <t>SP580</t>
@@ -481,9 +459,6 @@
     <t>2020.03.29</t>
   </si>
   <si>
-    <t>273K</t>
-  </si>
-  <si>
     <t>SP582</t>
   </si>
   <si>
@@ -559,26 +534,10 @@
     <t>5.4.0-k</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.39MB</t>
-    </r>
+    <t>72543e366645047dda549a18c64310d19313b5a8f9d60ba60a8b513ebb166fc5</t>
+  </si>
+  <si>
+    <t>487KB</t>
   </si>
   <si>
     <t>Intel</t>
@@ -639,7 +598,7 @@
     <t>13a4baf77f9ed7e26768b7702533f608b86c158514471dd01733ce154911aef6</t>
   </si>
   <si>
-    <t>2.4M</t>
+    <t>2.4MB</t>
   </si>
   <si>
     <t>SM330</t>
@@ -2079,10 +2038,10 @@
   <sheetPr/>
   <dimension ref="A1:R64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="M66" sqref="M66"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2092,10 +2051,10 @@
     <col min="3" max="3" width="8.75" style="10" customWidth="1"/>
     <col min="4" max="4" width="10.5" style="10" customWidth="1"/>
     <col min="5" max="5" width="10.25" style="10" customWidth="1"/>
-    <col min="6" max="6" width="27.5" style="10" customWidth="1"/>
-    <col min="7" max="7" width="15.25" style="10" customWidth="1"/>
-    <col min="8" max="8" width="11.375" style="10" customWidth="1"/>
-    <col min="9" max="9" width="11" style="10" customWidth="1"/>
+    <col min="6" max="6" width="21.125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="7.875" style="10" customWidth="1"/>
+    <col min="8" max="8" width="14.625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="7.75" style="10" customWidth="1"/>
     <col min="10" max="10" width="13.125" style="10" customWidth="1"/>
     <col min="11" max="11" width="8.625" style="10" customWidth="1"/>
     <col min="12" max="12" width="7.125" style="10" customWidth="1"/>
@@ -2103,7 +2062,7 @@
     <col min="14" max="14" width="13.25" style="10" customWidth="1"/>
     <col min="15" max="15" width="9.625" style="10" customWidth="1"/>
     <col min="16" max="16" width="10.375" style="11" customWidth="1"/>
-    <col min="17" max="17" width="54.875" style="10" customWidth="1"/>
+    <col min="17" max="17" width="12.375" style="10" customWidth="1"/>
     <col min="18" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
@@ -2568,8 +2527,8 @@
       <c r="K9" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="L9" s="23" t="s">
-        <v>68</v>
+      <c r="L9" s="21" t="s">
+        <v>61</v>
       </c>
       <c r="M9" s="23" t="s">
         <v>62</v>
@@ -2589,16 +2548,16 @@
     </row>
     <row r="10" s="6" customFormat="1" spans="1:17">
       <c r="A10" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="18" t="s">
         <v>69</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>70</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>22</v>
@@ -2607,49 +2566,49 @@
         <v>23</v>
       </c>
       <c r="G10" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="20" t="s">
         <v>72</v>
-      </c>
-      <c r="H10" s="20" t="s">
-        <v>73</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>58</v>
       </c>
       <c r="J10" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="K10" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="K10" s="6" t="s">
+      <c r="L10" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="L10" s="20" t="s">
+      <c r="M10" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="M10" s="20" t="s">
+      <c r="N10" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="N10" s="20" t="s">
+      <c r="O10" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="P10" s="20"/>
       <c r="Q10" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" s="6" customFormat="1" spans="1:17">
       <c r="A11" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C11" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>22</v>
@@ -2658,51 +2617,51 @@
         <v>23</v>
       </c>
       <c r="G11" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="H11" s="20" t="s">
-        <v>73</v>
-      </c>
       <c r="I11" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="J11" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="J11" s="20" t="s">
+      <c r="K11" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="L11" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="M11" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="N11" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="K11" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="L11" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="M11" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="N11" s="20" t="s">
+      <c r="O11" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="O11" s="20" t="s">
+      <c r="P11" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="P11" s="20" t="s">
-        <v>87</v>
-      </c>
       <c r="Q11" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" s="6" customFormat="1" spans="1:17">
       <c r="A12" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>22</v>
@@ -2711,51 +2670,51 @@
         <v>23</v>
       </c>
       <c r="G12" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="H12" s="20" t="s">
-        <v>73</v>
-      </c>
       <c r="I12" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J12" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="L12" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="M12" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="N12" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="K12" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="L12" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="M12" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="N12" s="20" t="s">
+      <c r="O12" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="P12" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="O12" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="P12" s="20" t="s">
-        <v>91</v>
-      </c>
       <c r="Q12" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" s="6" customFormat="1" spans="1:17">
       <c r="A13" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="18" t="s">
-        <v>70</v>
-      </c>
       <c r="C13" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>22</v>
@@ -2764,51 +2723,51 @@
         <v>23</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I13" s="20" t="s">
         <v>58</v>
       </c>
       <c r="J13" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="L13" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="M13" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="N13" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="K13" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="L13" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="M13" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="N13" s="20" t="s">
+      <c r="O13" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="P13" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="O13" s="6" t="s">
+      <c r="Q13" s="26" t="s">
         <v>79</v>
-      </c>
-      <c r="P13" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q13" s="26" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="14" s="6" customFormat="1" spans="1:17">
       <c r="A14" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E14" s="20" t="s">
         <v>22</v>
@@ -2817,51 +2776,51 @@
         <v>23</v>
       </c>
       <c r="G14" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14" s="20" t="s">
         <v>72</v>
-      </c>
-      <c r="H14" s="20" t="s">
-        <v>73</v>
       </c>
       <c r="I14" s="20" t="s">
         <v>58</v>
       </c>
       <c r="J14" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K14" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="L14" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="L14" s="20" t="s">
+      <c r="M14" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="M14" s="20" t="s">
-        <v>77</v>
-      </c>
       <c r="N14" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="O14" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="P14" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="O14" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="P14" s="20" t="s">
-        <v>99</v>
-      </c>
       <c r="Q14" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" s="6" customFormat="1" spans="1:17">
       <c r="A15" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E15" s="20" t="s">
         <v>22</v>
@@ -2870,51 +2829,51 @@
         <v>23</v>
       </c>
       <c r="G15" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" s="20" t="s">
         <v>72</v>
-      </c>
-      <c r="H15" s="20" t="s">
-        <v>73</v>
       </c>
       <c r="I15" s="20" t="s">
         <v>58</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K15" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="L15" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="L15" s="20" t="s">
+      <c r="M15" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="M15" s="20" t="s">
-        <v>77</v>
-      </c>
       <c r="N15" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="O15" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="P15" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="O15" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="P15" s="20" t="s">
-        <v>102</v>
-      </c>
       <c r="Q15" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" s="6" customFormat="1" spans="1:17">
       <c r="A16" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="C16" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" s="20" t="s">
         <v>104</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>105</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>22</v>
@@ -2923,37 +2882,37 @@
         <v>23</v>
       </c>
       <c r="G16" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="H16" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="H16" s="20" t="s">
+      <c r="I16" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="I16" s="20" t="s">
+      <c r="J16" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="J16" s="20" t="s">
+      <c r="K16" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="K16" s="20" t="s">
+      <c r="L16" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="L16" s="20" t="s">
+      <c r="M16" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="M16" s="20" t="s">
+      <c r="N16" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="N16" s="20" t="s">
+      <c r="O16" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="O16" s="20" t="s">
+      <c r="P16" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="P16" s="20" t="s">
+      <c r="Q16" s="26" t="s">
         <v>115</v>
-      </c>
-      <c r="Q16" s="26" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="17" s="6" customFormat="1" spans="1:17">
@@ -2961,13 +2920,13 @@
         <v>53</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C17" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E17" s="20" t="s">
         <v>22</v>
@@ -2976,37 +2935,37 @@
         <v>23</v>
       </c>
       <c r="G17" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="H17" s="20" t="s">
         <v>119</v>
-      </c>
-      <c r="H17" s="20" t="s">
-        <v>120</v>
       </c>
       <c r="I17" s="20" t="s">
         <v>26</v>
       </c>
       <c r="J17" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="K17" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="K17" s="20" t="s">
+      <c r="L17" s="20" t="s">
         <v>122</v>
-      </c>
-      <c r="L17" s="20" t="s">
-        <v>123</v>
       </c>
       <c r="M17" s="20" t="s">
         <v>62</v>
       </c>
       <c r="N17" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="O17" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="O17" s="8" t="s">
+      <c r="P17" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="P17" s="20" t="s">
+      <c r="Q17" s="26" t="s">
         <v>126</v>
-      </c>
-      <c r="Q17" s="26" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="18" s="6" customFormat="1" spans="1:17">
@@ -3014,13 +2973,13 @@
         <v>53</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C18" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E18" s="20" t="s">
         <v>22</v>
@@ -3029,35 +2988,35 @@
         <v>23</v>
       </c>
       <c r="G18" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="H18" s="20" t="s">
         <v>119</v>
-      </c>
-      <c r="H18" s="20" t="s">
-        <v>120</v>
       </c>
       <c r="I18" s="20" t="s">
         <v>26</v>
       </c>
       <c r="J18" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K18" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="L18" s="20" t="s">
         <v>122</v>
-      </c>
-      <c r="L18" s="20" t="s">
-        <v>123</v>
       </c>
       <c r="M18" s="20" t="s">
         <v>62</v>
       </c>
       <c r="N18" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O18" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P18" s="20"/>
       <c r="Q18" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" s="6" customFormat="1" spans="1:17">
@@ -3065,13 +3024,13 @@
         <v>53</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C19" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>22</v>
@@ -3080,10 +3039,10 @@
         <v>23</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H19" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I19" s="20" t="s">
         <v>58</v>
@@ -3092,23 +3051,23 @@
         <v>59</v>
       </c>
       <c r="K19" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="L19" s="20" t="s">
         <v>133</v>
-      </c>
-      <c r="L19" s="20" t="s">
-        <v>134</v>
       </c>
       <c r="M19" s="20" t="s">
         <v>62</v>
       </c>
       <c r="N19" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O19" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P19" s="20"/>
       <c r="Q19" s="26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" s="6" customFormat="1" spans="1:17">
@@ -3116,13 +3075,13 @@
         <v>53</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E20" s="20" t="s">
         <v>22</v>
@@ -3131,114 +3090,114 @@
         <v>23</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H20" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I20" s="20" t="s">
         <v>58</v>
       </c>
       <c r="J20" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K20" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="L20" s="20" t="s">
         <v>133</v>
-      </c>
-      <c r="L20" s="20" t="s">
-        <v>140</v>
       </c>
       <c r="M20" s="20" t="s">
         <v>62</v>
       </c>
       <c r="N20" s="20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="O20" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P20" s="20"/>
       <c r="Q20" s="26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" s="6" customFormat="1" spans="1:17">
       <c r="A21" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="18" t="s">
         <v>69</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>70</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D21" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21" s="20" t="s">
         <v>142</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="H21" s="20" t="s">
-        <v>144</v>
       </c>
       <c r="I21" s="20" t="s">
         <v>58</v>
       </c>
       <c r="J21" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K21" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="L21" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="M21" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="N21" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="L21" s="20" t="s">
+      <c r="O21" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="P21" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="M21" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="N21" s="20" t="s">
+      <c r="Q21" s="26" t="s">
         <v>147</v>
-      </c>
-      <c r="O21" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="P21" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q21" s="26" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="22" s="6" customFormat="1" spans="1:17">
       <c r="A22" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F22" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I22" s="20" t="s">
         <v>58</v>
@@ -3247,235 +3206,237 @@
         <v>46</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="L22" s="20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="M22" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N22" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="O22" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="P22" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="O22" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="P22" s="20" t="s">
-        <v>102</v>
-      </c>
       <c r="Q22" s="26" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" s="6" customFormat="1" spans="1:17">
       <c r="A23" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F23" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H23" s="20" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I23" s="20" t="s">
         <v>58</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K23" s="20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="L23" s="20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="M23" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N23" s="20" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="O23" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P23" s="20" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="Q23" s="26" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" s="6" customFormat="1" spans="1:17">
       <c r="A24" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F24" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H24" s="20" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I24" s="20" t="s">
         <v>58</v>
       </c>
       <c r="J24" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="K24" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="L24" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="M24" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="N24" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="O24" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="P24" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="K24" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="L24" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="M24" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="N24" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="O24" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="P24" s="20" t="s">
-        <v>155</v>
-      </c>
       <c r="Q24" s="26" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" s="6" customFormat="1" spans="1:17">
       <c r="A25" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F25" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G25" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H25" s="20" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I25" s="20" t="s">
         <v>58</v>
       </c>
       <c r="J25" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K25" s="20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="L25" s="20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="M25" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N25" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="O25" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="P25" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="O25" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="P25" s="20" t="s">
-        <v>160</v>
-      </c>
       <c r="Q25" s="26" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="D26" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="E26" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="F26" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="C26" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="D26" s="21" t="s">
+      <c r="H26" s="21" t="s">
         <v>163</v>
-      </c>
-      <c r="E26" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="F26" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="H26" s="21" t="s">
-        <v>165</v>
       </c>
       <c r="I26" s="21" t="s">
         <v>58</v>
       </c>
       <c r="J26" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="K26" s="21"/>
+        <v>108</v>
+      </c>
+      <c r="K26" s="21" t="s">
+        <v>164</v>
+      </c>
       <c r="L26" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="M26" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="M26" s="21" t="s">
+      <c r="N26" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="N26" s="21" t="s">
+      <c r="O26" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="O26" s="21" t="s">
+      <c r="P26" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="P26" s="21" t="s">
+      <c r="Q26" s="20" t="s">
         <v>170</v>
-      </c>
-      <c r="Q26" s="20" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -3489,19 +3450,19 @@
         <v>53</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F27" s="21" t="s">
         <v>23</v>
       </c>
       <c r="G27" s="21" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H27" s="21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I27" s="21" t="s">
         <v>58</v>
@@ -3509,21 +3470,23 @@
       <c r="J27" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="K27" s="21"/>
+      <c r="K27" s="21" t="s">
+        <v>164</v>
+      </c>
       <c r="L27" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="M27" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="M27" s="21" t="s">
-        <v>167</v>
-      </c>
       <c r="N27" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="O27" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="P27" s="21" t="s">
         <v>173</v>
-      </c>
-      <c r="O27" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="P27" s="21" t="s">
-        <v>174</v>
       </c>
       <c r="Q27" s="6" t="s">
         <v>66</v>
@@ -3540,46 +3503,46 @@
         <v>53</v>
       </c>
       <c r="D28" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="E28" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="F28" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G28" s="20" t="s">
+      <c r="H28" s="20" t="s">
         <v>176</v>
-      </c>
-      <c r="H28" s="20" t="s">
-        <v>177</v>
       </c>
       <c r="I28" s="20" t="s">
         <v>58</v>
       </c>
       <c r="J28" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="K28" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="K28" s="20" t="s">
+      <c r="L28" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="L28" s="20" t="s">
+      <c r="M28" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="N28" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="M28" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="N28" s="20" t="s">
+      <c r="O28" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="O28" s="20" t="s">
+      <c r="P28" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="P28" s="20" t="s">
+      <c r="Q28" s="26" t="s">
         <v>183</v>
-      </c>
-      <c r="Q28" s="26" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="29" s="6" customFormat="1" spans="1:17">
@@ -3587,52 +3550,52 @@
         <v>8086</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C29" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F29" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G29" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="H29" s="20" t="s">
         <v>176</v>
-      </c>
-      <c r="H29" s="20" t="s">
-        <v>177</v>
       </c>
       <c r="I29" s="20" t="s">
         <v>58</v>
       </c>
       <c r="J29" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="K29" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="L29" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="M29" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="N29" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="K29" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="L29" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="M29" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="N29" s="20" t="s">
+      <c r="O29" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="O29" s="20" t="s">
+      <c r="P29" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="P29" s="20" t="s">
-        <v>190</v>
-      </c>
       <c r="Q29" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="30" s="6" customFormat="1" spans="1:17">
@@ -3640,52 +3603,52 @@
         <v>8086</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C30" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F30" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G30" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="H30" s="20" t="s">
         <v>176</v>
-      </c>
-      <c r="H30" s="20" t="s">
-        <v>177</v>
       </c>
       <c r="I30" s="20" t="s">
         <v>58</v>
       </c>
       <c r="J30" s="20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K30" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="L30" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="L30" s="20" t="s">
-        <v>180</v>
-      </c>
       <c r="M30" s="20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N30" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="O30" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="O30" s="20" t="s">
+      <c r="P30" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="P30" s="20" t="s">
-        <v>190</v>
-      </c>
       <c r="Q30" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="31" s="6" customFormat="1" spans="1:17">
@@ -3693,52 +3656,52 @@
         <v>8086</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C31" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F31" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G31" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="H31" s="20" t="s">
         <v>176</v>
-      </c>
-      <c r="H31" s="20" t="s">
-        <v>177</v>
       </c>
       <c r="I31" s="20" t="s">
         <v>58</v>
       </c>
       <c r="J31" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="K31" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="K31" s="20" t="s">
+      <c r="L31" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="L31" s="20" t="s">
-        <v>180</v>
-      </c>
       <c r="M31" s="20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N31" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="O31" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="O31" s="20" t="s">
+      <c r="P31" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="P31" s="20" t="s">
-        <v>190</v>
-      </c>
       <c r="Q31" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="32" s="6" customFormat="1" spans="1:17">
@@ -3746,52 +3709,52 @@
         <v>8086</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C32" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F32" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G32" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="H32" s="20" t="s">
         <v>176</v>
-      </c>
-      <c r="H32" s="20" t="s">
-        <v>177</v>
       </c>
       <c r="I32" s="20" t="s">
         <v>58</v>
       </c>
       <c r="J32" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K32" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="L32" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="L32" s="20" t="s">
-        <v>180</v>
-      </c>
       <c r="M32" s="20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N32" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="O32" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="O32" s="20" t="s">
+      <c r="P32" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="P32" s="20" t="s">
-        <v>190</v>
-      </c>
       <c r="Q32" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="33" s="6" customFormat="1" spans="1:17">
@@ -3805,46 +3768,46 @@
         <v>53</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F33" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G33" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="H33" s="20" t="s">
         <v>176</v>
-      </c>
-      <c r="H33" s="20" t="s">
-        <v>177</v>
       </c>
       <c r="I33" s="20" t="s">
         <v>58</v>
       </c>
       <c r="J33" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K33" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L33" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="M33" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="N33" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="M33" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="N33" s="20" t="s">
+      <c r="O33" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="P33" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="O33" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="P33" s="20" t="s">
-        <v>200</v>
-      </c>
       <c r="Q33" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="34" s="6" customFormat="1" spans="1:17">
@@ -3852,52 +3815,52 @@
         <v>1000</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C34" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D34" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="H34" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="I34" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="J34" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="K34" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="E34" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="F34" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G34" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="H34" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="I34" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="J34" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="K34" s="20" t="s">
+      <c r="L34" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="L34" s="20" t="s">
+      <c r="M34" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="N34" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="M34" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="N34" s="20" t="s">
+      <c r="O34" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="O34" s="20" t="s">
+      <c r="P34" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="P34" s="20" t="s">
+      <c r="Q34" s="26" t="s">
         <v>207</v>
-      </c>
-      <c r="Q34" s="26" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="35" s="6" customFormat="1" spans="1:17">
@@ -3905,52 +3868,52 @@
         <v>1000</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D35" s="20">
         <v>9361</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G35" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="H35" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="H35" s="20" t="s">
+      <c r="I35" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="I35" s="20" t="s">
-        <v>108</v>
-      </c>
       <c r="J35" s="20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K35" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="L35" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="L35" s="20" t="s">
-        <v>204</v>
-      </c>
       <c r="M35" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N35" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="O35" s="20" t="s">
         <v>210</v>
       </c>
-      <c r="O35" s="20" t="s">
+      <c r="P35" s="20" t="s">
         <v>211</v>
       </c>
-      <c r="P35" s="20" t="s">
-        <v>212</v>
-      </c>
       <c r="Q35" s="26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="36" s="6" customFormat="1" spans="1:17">
@@ -3958,52 +3921,52 @@
         <v>1000</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C36" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D36" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="H36" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="I36" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="J36" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="K36" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="L36" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="M36" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="N36" s="20" t="s">
         <v>213</v>
       </c>
-      <c r="E36" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="F36" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G36" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="H36" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="I36" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="J36" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="K36" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="L36" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="M36" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="N36" s="20" t="s">
+      <c r="O36" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="P36" s="20" t="s">
         <v>214</v>
       </c>
-      <c r="O36" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="P36" s="20" t="s">
-        <v>215</v>
-      </c>
       <c r="Q36" s="26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" s="6" customFormat="1" spans="1:17">
@@ -4011,52 +3974,52 @@
         <v>1000</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C37" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F37" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G37" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="H37" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="H37" s="20" t="s">
+      <c r="I37" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="I37" s="20" t="s">
-        <v>108</v>
-      </c>
       <c r="J37" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K37" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="L37" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="L37" s="20" t="s">
-        <v>204</v>
-      </c>
       <c r="M37" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N37" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="O37" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="P37" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="O37" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="P37" s="20" t="s">
-        <v>217</v>
-      </c>
       <c r="Q37" s="26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="38" s="6" customFormat="1" spans="1:17">
@@ -4064,52 +4027,52 @@
         <v>1000</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D38" s="20">
         <v>9440</v>
       </c>
       <c r="E38" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F38" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G38" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="H38" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="H38" s="20" t="s">
+      <c r="I38" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="I38" s="20" t="s">
-        <v>108</v>
-      </c>
       <c r="J38" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K38" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="L38" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="L38" s="20" t="s">
-        <v>204</v>
-      </c>
       <c r="M38" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="N38" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="N38" s="20" t="s">
+      <c r="O38" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="O38" s="20" t="s">
+      <c r="P38" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="P38" s="20" t="s">
-        <v>115</v>
-      </c>
       <c r="Q38" s="26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="39" s="6" customFormat="1" spans="1:17">
@@ -4117,52 +4080,52 @@
         <v>1000</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C39" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D39" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F39" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="H39" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="I39" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="J39" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="K39" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="L39" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="M39" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="N39" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="E39" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="F39" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G39" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="H39" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="I39" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="J39" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="K39" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="L39" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="M39" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="N39" s="20" t="s">
+      <c r="O39" s="20" t="s">
         <v>220</v>
       </c>
-      <c r="O39" s="20" t="s">
+      <c r="P39" s="20" t="s">
         <v>221</v>
       </c>
-      <c r="P39" s="20" t="s">
-        <v>222</v>
-      </c>
       <c r="Q39" s="26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="40" s="6" customFormat="1" spans="1:17">
@@ -4170,52 +4133,52 @@
         <v>1000</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C40" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E40" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F40" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G40" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="H40" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="H40" s="20" t="s">
+      <c r="I40" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="I40" s="20" t="s">
+      <c r="J40" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="J40" s="20" t="s">
-        <v>109</v>
-      </c>
       <c r="K40" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="L40" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="L40" s="20" t="s">
-        <v>204</v>
-      </c>
       <c r="M40" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N40" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="O40" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="P40" s="20" t="s">
         <v>223</v>
       </c>
-      <c r="O40" s="20" t="s">
-        <v>221</v>
-      </c>
-      <c r="P40" s="20" t="s">
-        <v>224</v>
-      </c>
       <c r="Q40" s="26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="41" s="6" customFormat="1" spans="1:17">
@@ -4223,52 +4186,52 @@
         <v>1000</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C41" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D41" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="H41" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="I41" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="J41" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="K41" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="L41" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="M41" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="N41" s="20" t="s">
         <v>226</v>
       </c>
-      <c r="E41" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="F41" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G41" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="H41" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="I41" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="J41" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="K41" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="L41" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="M41" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="N41" s="20" t="s">
+      <c r="O41" s="20" t="s">
         <v>227</v>
       </c>
-      <c r="O41" s="20" t="s">
+      <c r="P41" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="P41" s="20" t="s">
-        <v>229</v>
-      </c>
       <c r="Q41" s="26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="42" s="8" customFormat="1" spans="1:17">
@@ -4276,13 +4239,13 @@
         <v>1000</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C42" s="19" t="s">
         <v>53</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>22</v>
@@ -4291,51 +4254,51 @@
         <v>23</v>
       </c>
       <c r="G42" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="H42" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="H42" s="6" t="s">
+      <c r="I42" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="I42" s="25" t="s">
-        <v>108</v>
-      </c>
       <c r="J42" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="K42" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="L42" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="M42" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="N42" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="O42" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="P42" s="18" t="s">
         <v>230</v>
       </c>
-      <c r="K42" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="L42" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="M42" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="N42" s="20" t="s">
-        <v>227</v>
-      </c>
-      <c r="O42" s="20" t="s">
-        <v>228</v>
-      </c>
-      <c r="P42" s="18" t="s">
+      <c r="Q42" s="26" t="s">
         <v>231</v>
-      </c>
-      <c r="Q42" s="26" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="43" s="6" customFormat="1" spans="1:17">
       <c r="A43" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="B43" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="B43" s="19" t="s">
-        <v>234</v>
-      </c>
       <c r="C43" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="D43" s="6" t="s">
         <v>233</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>234</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>22</v>
@@ -4344,49 +4307,49 @@
         <v>23</v>
       </c>
       <c r="G43" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="H43" s="20" t="s">
         <v>235</v>
-      </c>
-      <c r="H43" s="20" t="s">
-        <v>236</v>
       </c>
       <c r="I43" s="6" t="s">
         <v>26</v>
       </c>
       <c r="J43" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="K43" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="K43" s="6" t="s">
+      <c r="L43" s="20" t="s">
         <v>238</v>
       </c>
-      <c r="L43" s="20" t="s">
+      <c r="M43" s="20" t="s">
         <v>239</v>
       </c>
-      <c r="M43" s="20" t="s">
+      <c r="N43" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="N43" s="20" t="s">
+      <c r="O43" s="6" t="s">
         <v>241</v>
-      </c>
-      <c r="O43" s="6" t="s">
-        <v>242</v>
       </c>
       <c r="P43" s="18"/>
       <c r="Q43" s="26" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="44" s="9" customFormat="1" ht="14.45" customHeight="1" spans="1:17">
       <c r="A44" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="B44" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="B44" s="18" t="s">
-        <v>234</v>
-      </c>
       <c r="C44" s="20" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E44" s="20" t="s">
         <v>22</v>
@@ -4395,49 +4358,49 @@
         <v>23</v>
       </c>
       <c r="G44" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="H44" s="20" t="s">
         <v>235</v>
-      </c>
-      <c r="H44" s="20" t="s">
-        <v>236</v>
       </c>
       <c r="I44" s="20" t="s">
         <v>26</v>
       </c>
       <c r="J44" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K44" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="L44" s="20" t="s">
         <v>238</v>
       </c>
-      <c r="L44" s="20" t="s">
+      <c r="M44" s="20" t="s">
         <v>239</v>
       </c>
-      <c r="M44" s="20" t="s">
+      <c r="N44" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="N44" s="20" t="s">
+      <c r="O44" s="6" t="s">
         <v>241</v>
-      </c>
-      <c r="O44" s="6" t="s">
-        <v>242</v>
       </c>
       <c r="P44" s="20"/>
       <c r="Q44" s="26" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="45" s="6" customFormat="1" spans="1:17">
       <c r="A45" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="B45" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="B45" s="19" t="s">
-        <v>234</v>
-      </c>
       <c r="C45" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>22</v>
@@ -4446,49 +4409,49 @@
         <v>23</v>
       </c>
       <c r="G45" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="H45" s="20" t="s">
         <v>235</v>
-      </c>
-      <c r="H45" s="20" t="s">
-        <v>236</v>
       </c>
       <c r="I45" s="20" t="s">
         <v>26</v>
       </c>
       <c r="J45" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="K45" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="L45" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="M45" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="N45" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="K45" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="L45" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="M45" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="N45" s="6" t="s">
-        <v>247</v>
-      </c>
       <c r="O45" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P45" s="19"/>
       <c r="Q45" s="26" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="46" s="6" customFormat="1" spans="1:17">
       <c r="A46" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="B46" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="B46" s="19" t="s">
-        <v>234</v>
-      </c>
       <c r="C46" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>22</v>
@@ -4497,35 +4460,35 @@
         <v>23</v>
       </c>
       <c r="G46" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="H46" s="20" t="s">
         <v>235</v>
-      </c>
-      <c r="H46" s="20" t="s">
-        <v>236</v>
       </c>
       <c r="I46" s="20" t="s">
         <v>26</v>
       </c>
       <c r="J46" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K46" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="L46" s="20" t="s">
         <v>238</v>
       </c>
-      <c r="L46" s="20" t="s">
+      <c r="M46" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="M46" s="6" t="s">
-        <v>240</v>
-      </c>
       <c r="N46" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="O46" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P46" s="19"/>
       <c r="Q46" s="26" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="47" s="6" customFormat="1" spans="1:17">
@@ -4533,50 +4496,50 @@
         <v>1000</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C47" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E47" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F47" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G47" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="H47" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="H47" s="20" t="s">
+      <c r="I47" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="I47" s="20" t="s">
-        <v>108</v>
-      </c>
       <c r="J47" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K47" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="L47" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="L47" s="20" t="s">
-        <v>204</v>
-      </c>
       <c r="M47" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N47" s="20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O47" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P47" s="20"/>
       <c r="Q47" s="26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="48" s="6" customFormat="1" spans="1:17">
@@ -4584,50 +4547,50 @@
         <v>1000</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C48" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E48" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F48" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G48" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="H48" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="H48" s="20" t="s">
+      <c r="I48" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="I48" s="20" t="s">
-        <v>108</v>
-      </c>
       <c r="J48" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K48" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="L48" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="L48" s="20" t="s">
-        <v>204</v>
-      </c>
       <c r="M48" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N48" s="20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O48" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P48" s="20"/>
       <c r="Q48" s="26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="49" s="6" customFormat="1" spans="1:17">
@@ -4635,50 +4598,50 @@
         <v>1000</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C49" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E49" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F49" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G49" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="H49" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="H49" s="20" t="s">
+      <c r="I49" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="I49" s="20" t="s">
-        <v>108</v>
-      </c>
       <c r="J49" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K49" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="L49" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="L49" s="20" t="s">
-        <v>204</v>
-      </c>
       <c r="M49" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N49" s="20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O49" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P49" s="20"/>
       <c r="Q49" s="26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="50" s="6" customFormat="1" spans="1:17">
@@ -4686,50 +4649,50 @@
         <v>1000</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C50" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D50" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="E50" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F50" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G50" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="H50" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="I50" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="J50" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="K50" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="L50" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="M50" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="N50" s="20" t="s">
         <v>253</v>
       </c>
-      <c r="E50" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="F50" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G50" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="H50" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="I50" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="J50" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="K50" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="L50" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="M50" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="N50" s="20" t="s">
-        <v>254</v>
-      </c>
       <c r="O50" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P50" s="20"/>
       <c r="Q50" s="26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="51" s="6" customFormat="1" spans="1:17">
@@ -4737,64 +4700,64 @@
         <v>1000</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C51" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D51" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="E51" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F51" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G51" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="H51" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="I51" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="J51" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="K51" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="L51" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="M51" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="N51" s="20" t="s">
         <v>255</v>
       </c>
-      <c r="E51" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="F51" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G51" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="H51" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="I51" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="J51" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="K51" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="L51" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="M51" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="N51" s="20" t="s">
-        <v>256</v>
-      </c>
       <c r="O51" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P51" s="20"/>
       <c r="Q51" s="26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="52" s="6" customFormat="1" spans="1:17">
       <c r="A52" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" s="19" t="s">
         <v>103</v>
-      </c>
-      <c r="B52" s="19" t="s">
-        <v>104</v>
       </c>
       <c r="C52" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>22</v>
@@ -4803,51 +4766,51 @@
         <v>23</v>
       </c>
       <c r="G52" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H52" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="I52" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="J52" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="I52" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="J52" s="6" t="s">
+      <c r="K52" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="K52" s="6" t="s">
+      <c r="L52" s="20" t="s">
         <v>260</v>
       </c>
-      <c r="L52" s="20" t="s">
+      <c r="M52" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="N52" s="20" t="s">
         <v>261</v>
       </c>
-      <c r="M52" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="N52" s="20" t="s">
+      <c r="O52" s="20" t="s">
         <v>262</v>
       </c>
-      <c r="O52" s="20" t="s">
+      <c r="P52" s="18" t="s">
         <v>263</v>
       </c>
-      <c r="P52" s="18" t="s">
+      <c r="Q52" s="26" t="s">
         <v>264</v>
-      </c>
-      <c r="Q52" s="26" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="53" s="6" customFormat="1" spans="1:17">
       <c r="A53" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B53" s="19" t="s">
         <v>103</v>
-      </c>
-      <c r="B53" s="19" t="s">
-        <v>104</v>
       </c>
       <c r="C53" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>22</v>
@@ -4856,49 +4819,49 @@
         <v>23</v>
       </c>
       <c r="G53" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H53" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="I53" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="J53" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="I53" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="J53" s="6" t="s">
+      <c r="K53" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="K53" s="6" t="s">
+      <c r="L53" s="20" t="s">
         <v>260</v>
       </c>
-      <c r="L53" s="20" t="s">
-        <v>261</v>
-      </c>
       <c r="M53" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N53" s="20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O53" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="P53" s="18"/>
       <c r="Q53" s="26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="54" s="6" customFormat="1" spans="1:17">
       <c r="A54" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" s="19" t="s">
         <v>103</v>
-      </c>
-      <c r="B54" s="19" t="s">
-        <v>104</v>
       </c>
       <c r="C54" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>22</v>
@@ -4907,35 +4870,35 @@
         <v>23</v>
       </c>
       <c r="G54" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H54" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="I54" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="J54" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="I54" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="J54" s="6" t="s">
+      <c r="K54" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="K54" s="6" t="s">
+      <c r="L54" s="20" t="s">
         <v>260</v>
       </c>
-      <c r="L54" s="20" t="s">
-        <v>261</v>
-      </c>
       <c r="M54" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N54" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="O54" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="P54" s="18"/>
       <c r="Q54" s="26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="55" s="6" customFormat="1" spans="1:17">
@@ -4943,13 +4906,13 @@
         <v>53</v>
       </c>
       <c r="B55" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="C55" s="20" t="s">
         <v>268</v>
       </c>
-      <c r="C55" s="20" t="s">
+      <c r="D55" s="20" t="s">
         <v>269</v>
-      </c>
-      <c r="D55" s="20" t="s">
-        <v>270</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>22</v>
@@ -4958,32 +4921,32 @@
         <v>23</v>
       </c>
       <c r="G55" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="I55" s="20" t="s">
         <v>271</v>
       </c>
-      <c r="I55" s="20" t="s">
+      <c r="J55" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="J55" s="20" t="s">
+      <c r="K55" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="K55" s="6" t="s">
+      <c r="L55" s="6" t="s">
         <v>274</v>
-      </c>
-      <c r="L55" s="6" t="s">
-        <v>275</v>
       </c>
       <c r="M55" s="20" t="s">
         <v>62</v>
       </c>
       <c r="N55" s="20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="O55" s="20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="P55" s="19"/>
       <c r="Q55" s="26" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="56" s="6" customFormat="1" spans="1:17">
@@ -4991,47 +4954,47 @@
         <v>53</v>
       </c>
       <c r="B56" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="C56" s="20" t="s">
         <v>268</v>
       </c>
-      <c r="C56" s="20" t="s">
+      <c r="D56" s="20" t="s">
         <v>269</v>
       </c>
-      <c r="D56" s="20" t="s">
+      <c r="E56" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G56" s="20" t="s">
         <v>270</v>
       </c>
-      <c r="E56" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G56" s="20" t="s">
+      <c r="I56" s="20" t="s">
         <v>271</v>
       </c>
-      <c r="I56" s="20" t="s">
+      <c r="J56" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="J56" s="20" t="s">
+      <c r="K56" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="K56" s="6" t="s">
+      <c r="L56" s="6" t="s">
         <v>274</v>
-      </c>
-      <c r="L56" s="6" t="s">
-        <v>275</v>
       </c>
       <c r="M56" s="20" t="s">
         <v>62</v>
       </c>
       <c r="N56" s="20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="O56" s="20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="P56" s="19"/>
       <c r="Q56" s="26" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="57" s="6" customFormat="1" spans="1:17">
@@ -5039,13 +5002,13 @@
         <v>53</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C57" s="20" t="s">
+        <v>268</v>
+      </c>
+      <c r="D57" s="20" t="s">
         <v>269</v>
-      </c>
-      <c r="D57" s="20" t="s">
-        <v>270</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>22</v>
@@ -5054,32 +5017,32 @@
         <v>23</v>
       </c>
       <c r="G57" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="I57" s="20" t="s">
         <v>271</v>
       </c>
-      <c r="I57" s="20" t="s">
+      <c r="J57" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="J57" s="20" t="s">
-        <v>273</v>
-      </c>
       <c r="K57" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L57" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="M57" s="20" t="s">
         <v>62</v>
       </c>
       <c r="N57" s="20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="O57" s="20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="P57" s="19"/>
       <c r="Q57" s="26" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="58" s="6" customFormat="1" spans="1:17">
@@ -5087,47 +5050,47 @@
         <v>53</v>
       </c>
       <c r="B58" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="C58" s="20" t="s">
+        <v>268</v>
+      </c>
+      <c r="D58" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="E58" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G58" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="I58" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="J58" s="20" t="s">
+        <v>272</v>
+      </c>
+      <c r="K58" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="C58" s="20" t="s">
-        <v>269</v>
-      </c>
-      <c r="D58" s="20" t="s">
-        <v>270</v>
-      </c>
-      <c r="E58" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G58" s="20" t="s">
-        <v>271</v>
-      </c>
-      <c r="I58" s="20" t="s">
-        <v>272</v>
-      </c>
-      <c r="J58" s="20" t="s">
-        <v>273</v>
-      </c>
-      <c r="K58" s="6" t="s">
-        <v>279</v>
-      </c>
       <c r="L58" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="M58" s="20" t="s">
         <v>62</v>
       </c>
       <c r="N58" s="20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="O58" s="20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="P58" s="19"/>
       <c r="Q58" s="26" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="59" s="6" customFormat="1" spans="1:17">
@@ -5135,13 +5098,13 @@
         <v>53</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C59" s="20" t="s">
+        <v>268</v>
+      </c>
+      <c r="D59" s="20" t="s">
         <v>269</v>
-      </c>
-      <c r="D59" s="20" t="s">
-        <v>270</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>22</v>
@@ -5150,34 +5113,34 @@
         <v>23</v>
       </c>
       <c r="G59" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="I59" s="20" t="s">
         <v>271</v>
       </c>
-      <c r="I59" s="20" t="s">
+      <c r="J59" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="J59" s="20" t="s">
-        <v>273</v>
-      </c>
       <c r="K59" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L59" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="M59" s="20" t="s">
         <v>62</v>
       </c>
       <c r="N59" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="O59" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="P59" s="18" t="s">
         <v>284</v>
       </c>
-      <c r="O59" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="P59" s="18" t="s">
+      <c r="Q59" s="26" t="s">
         <v>285</v>
-      </c>
-      <c r="Q59" s="26" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="60" s="6" customFormat="1" spans="1:17">
@@ -5185,49 +5148,49 @@
         <v>53</v>
       </c>
       <c r="B60" s="18" t="s">
+        <v>281</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>268</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="E60" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G60" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="I60" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="J60" s="20" t="s">
+        <v>272</v>
+      </c>
+      <c r="K60" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="C60" s="20" t="s">
-        <v>269</v>
-      </c>
-      <c r="D60" s="20" t="s">
-        <v>270</v>
-      </c>
-      <c r="E60" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G60" s="20" t="s">
-        <v>271</v>
-      </c>
-      <c r="I60" s="20" t="s">
-        <v>272</v>
-      </c>
-      <c r="J60" s="20" t="s">
-        <v>273</v>
-      </c>
-      <c r="K60" s="6" t="s">
-        <v>283</v>
-      </c>
       <c r="L60" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="M60" s="20" t="s">
         <v>62</v>
       </c>
       <c r="N60" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="O60" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="P60" s="18" t="s">
         <v>284</v>
       </c>
-      <c r="O60" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="P60" s="18" t="s">
+      <c r="Q60" s="26" t="s">
         <v>285</v>
-      </c>
-      <c r="Q60" s="26" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="61" s="6" customFormat="1" spans="1:17">
@@ -5235,13 +5198,13 @@
         <v>53</v>
       </c>
       <c r="B61" s="18" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C61" s="20" t="s">
+        <v>268</v>
+      </c>
+      <c r="D61" s="20" t="s">
         <v>269</v>
-      </c>
-      <c r="D61" s="20" t="s">
-        <v>270</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>22</v>
@@ -5250,34 +5213,34 @@
         <v>23</v>
       </c>
       <c r="G61" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="I61" s="20" t="s">
         <v>271</v>
       </c>
-      <c r="I61" s="20" t="s">
+      <c r="J61" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="J61" s="20" t="s">
-        <v>273</v>
-      </c>
       <c r="K61" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L61" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="M61" s="20" t="s">
         <v>62</v>
       </c>
       <c r="N61" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="O61" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="P61" s="18" t="s">
         <v>287</v>
       </c>
-      <c r="O61" s="20" t="s">
-        <v>287</v>
-      </c>
-      <c r="P61" s="18" t="s">
-        <v>288</v>
-      </c>
       <c r="Q61" s="26" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="62" s="6" customFormat="1" spans="1:17">
@@ -5285,49 +5248,49 @@
         <v>53</v>
       </c>
       <c r="B62" s="18" t="s">
+        <v>281</v>
+      </c>
+      <c r="C62" s="20" t="s">
+        <v>268</v>
+      </c>
+      <c r="D62" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="E62" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G62" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="I62" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="J62" s="20" t="s">
+        <v>272</v>
+      </c>
+      <c r="K62" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="C62" s="20" t="s">
-        <v>269</v>
-      </c>
-      <c r="D62" s="20" t="s">
-        <v>270</v>
-      </c>
-      <c r="E62" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G62" s="20" t="s">
-        <v>271</v>
-      </c>
-      <c r="I62" s="20" t="s">
-        <v>272</v>
-      </c>
-      <c r="J62" s="20" t="s">
-        <v>273</v>
-      </c>
-      <c r="K62" s="6" t="s">
-        <v>283</v>
-      </c>
       <c r="L62" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="M62" s="20" t="s">
         <v>62</v>
       </c>
       <c r="N62" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="O62" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="P62" s="18" t="s">
         <v>287</v>
       </c>
-      <c r="O62" s="20" t="s">
-        <v>287</v>
-      </c>
-      <c r="P62" s="18" t="s">
-        <v>288</v>
-      </c>
       <c r="Q62" s="26" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="63" s="6" customFormat="1" spans="2:16">

</xml_diff>

<commit_message>
1.add 54 card infomation 2.add 12 Mcx653105A-HDATA integrated card info.
</commit_message>
<xml_diff>
--- a/data/compatibility/openEuler20.03-LTS上两类平台板卡兼容清单.xlsx
+++ b/data/compatibility/openEuler20.03-LTS上两类平台板卡兼容清单.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20925" windowHeight="9750" tabRatio="603"/>
+    <workbookView windowWidth="24225" windowHeight="12450" tabRatio="603"/>
   </bookViews>
   <sheets>
     <sheet name="openEuler20.03-LTS两类平台板卡兼容性" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'openEuler20.03-LTS两类平台板卡兼容性'!$A$1:$Q$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'openEuler20.03-LTS两类平台板卡兼容性'!$A$1:$Q$92</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="322">
   <si>
     <t>vendorID</t>
   </si>
@@ -961,6 +961,108 @@
   </si>
   <si>
     <t>02313SHF/02314BCJ</t>
+  </si>
+  <si>
+    <t>d130</t>
+  </si>
+  <si>
+    <t>5.1-2.5.2</t>
+  </si>
+  <si>
+    <t>2021.3.19</t>
+  </si>
+  <si>
+    <t>242M</t>
+  </si>
+  <si>
+    <t>SP380</t>
+  </si>
+  <si>
+    <t>03025SNT</t>
+  </si>
+  <si>
+    <t>d129</t>
+  </si>
+  <si>
+    <t>2.3.2.16</t>
+  </si>
+  <si>
+    <t>2020.12.28</t>
+  </si>
+  <si>
+    <t>46c24833a2c753df7ddc1e9624e0552201967111aa62280036c691547a9eb058</t>
+  </si>
+  <si>
+    <t>830K</t>
+  </si>
+  <si>
+    <t>SP570</t>
+  </si>
+  <si>
+    <t>02312BWF</t>
+  </si>
+  <si>
+    <t>07.706.03.00-rc1</t>
+  </si>
+  <si>
+    <t>32a528f2885b12a9d6cacfe58a33c044ad73a2b50a83f78704fec4d83c2a55c9</t>
+  </si>
+  <si>
+    <t>293K</t>
+  </si>
+  <si>
+    <t>009c</t>
+  </si>
+  <si>
+    <t>MCX4121A-ACAT</t>
+  </si>
+  <si>
+    <t>06310106</t>
+  </si>
+  <si>
+    <t>0020</t>
+  </si>
+  <si>
+    <t>MCX512A-ACAT</t>
+  </si>
+  <si>
+    <t>ConnectX-5</t>
+  </si>
+  <si>
+    <t>06310156</t>
+  </si>
+  <si>
+    <t>0006</t>
+  </si>
+  <si>
+    <t>MCX515A-CCAT</t>
+  </si>
+  <si>
+    <t>06310149</t>
+  </si>
+  <si>
+    <t>1.9.38.8</t>
+  </si>
+  <si>
+    <t>163K</t>
+  </si>
+  <si>
+    <t>TM210</t>
+  </si>
+  <si>
+    <t>1521</t>
+  </si>
+  <si>
+    <t>1f24</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>2022.05.10</t>
+  </si>
+  <si>
+    <t>XP210</t>
   </si>
 </sst>
 </file>
@@ -1622,7 +1724,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="50">
       <alignment vertical="center"/>
@@ -1645,6 +1747,10 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2036,86 +2142,86 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:R64"/>
+  <dimension ref="A1:R93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="10.625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="8.75" style="10" customWidth="1"/>
-    <col min="4" max="4" width="10.5" style="10" customWidth="1"/>
-    <col min="5" max="5" width="10.25" style="10" customWidth="1"/>
-    <col min="6" max="6" width="21.125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="7.875" style="10" customWidth="1"/>
-    <col min="8" max="8" width="14.625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="7.75" style="10" customWidth="1"/>
-    <col min="10" max="10" width="13.125" style="10" customWidth="1"/>
-    <col min="11" max="11" width="8.625" style="10" customWidth="1"/>
-    <col min="12" max="12" width="7.125" style="10" customWidth="1"/>
-    <col min="13" max="13" width="7.875" style="10" customWidth="1"/>
-    <col min="14" max="14" width="13.25" style="10" customWidth="1"/>
-    <col min="15" max="15" width="9.625" style="10" customWidth="1"/>
-    <col min="16" max="16" width="10.375" style="11" customWidth="1"/>
-    <col min="17" max="17" width="12.375" style="10" customWidth="1"/>
-    <col min="18" max="16384" width="9" style="10"/>
+    <col min="1" max="1" width="11.125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="10.625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="8.75" style="12" customWidth="1"/>
+    <col min="4" max="4" width="10.5" style="12" customWidth="1"/>
+    <col min="5" max="5" width="10.25" style="12" customWidth="1"/>
+    <col min="6" max="6" width="29.875" style="12" customWidth="1"/>
+    <col min="7" max="7" width="14.5" style="12" customWidth="1"/>
+    <col min="8" max="8" width="14.625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="7.75" style="12" customWidth="1"/>
+    <col min="10" max="10" width="13.125" style="12" customWidth="1"/>
+    <col min="11" max="11" width="11.75" style="12" customWidth="1"/>
+    <col min="12" max="12" width="7.125" style="12" customWidth="1"/>
+    <col min="13" max="13" width="7.875" style="12" customWidth="1"/>
+    <col min="14" max="14" width="13.25" style="12" customWidth="1"/>
+    <col min="15" max="15" width="9.625" style="12" customWidth="1"/>
+    <col min="16" max="16" width="10.375" style="13" customWidth="1"/>
+    <col min="17" max="17" width="156.625" style="12" customWidth="1"/>
+    <col min="18" max="16384" width="9" style="12"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="1" ht="20.25" customHeight="1" spans="1:18">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="Q1" s="16" t="s">
         <v>16</v>
       </c>
       <c r="R1" s="4" t="s">
@@ -2126,7 +2232,7 @@
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="19" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -2168,7 +2274,7 @@
       <c r="O2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="P2" s="17" t="s">
+      <c r="P2" s="19" t="s">
         <v>18</v>
       </c>
       <c r="Q2" s="5" t="s">
@@ -2179,13 +2285,13 @@
       <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="21">
         <v>1077</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="22" t="s">
         <v>21</v>
       </c>
       <c r="E3" s="6" t="s">
@@ -2194,37 +2300,37 @@
       <c r="F3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="22" t="s">
         <v>27</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="20" t="s">
+      <c r="M3" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="20" t="s">
+      <c r="N3" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="20" t="s">
+      <c r="O3" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="P3" s="18" t="s">
+      <c r="P3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="Q3" s="26" t="s">
+      <c r="Q3" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2232,10 +2338,10 @@
       <c r="A4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="21">
         <v>1077</v>
       </c>
       <c r="D4" s="6" t="s">
@@ -2247,37 +2353,37 @@
       <c r="F4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="H4" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="20" t="s">
+      <c r="I4" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="20" t="s">
+      <c r="J4" s="22" t="s">
         <v>37</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="20" t="s">
+      <c r="L4" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="20" t="s">
+      <c r="M4" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="N4" s="20" t="s">
+      <c r="N4" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="O4" s="20" t="s">
+      <c r="O4" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="P4" s="18" t="s">
+      <c r="P4" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="Q4" s="26" t="s">
+      <c r="Q4" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2285,10 +2391,10 @@
       <c r="A5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="21">
         <v>1077</v>
       </c>
       <c r="D5" s="6" t="s">
@@ -2300,37 +2406,37 @@
       <c r="F5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="I5" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="J5" s="22" t="s">
         <v>42</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="L5" s="20" t="s">
+      <c r="L5" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="M5" s="20" t="s">
+      <c r="M5" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="N5" s="20" t="s">
+      <c r="N5" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="O5" s="20" t="s">
+      <c r="O5" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="P5" s="18" t="s">
+      <c r="P5" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="Q5" s="26" t="s">
+      <c r="Q5" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2338,10 +2444,10 @@
       <c r="A6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="21">
         <v>1077</v>
       </c>
       <c r="D6" s="6" t="s">
@@ -2353,37 +2459,37 @@
       <c r="F6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="H6" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="20" t="s">
+      <c r="J6" s="22" t="s">
         <v>46</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="L6" s="20" t="s">
+      <c r="L6" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="M6" s="20" t="s">
+      <c r="M6" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="N6" s="20" t="s">
+      <c r="N6" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="O6" s="20" t="s">
+      <c r="O6" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="P6" s="18" t="s">
+      <c r="P6" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="Q6" s="26" t="s">
+      <c r="Q6" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2391,10 +2497,10 @@
       <c r="A7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="21">
         <v>1077</v>
       </c>
       <c r="D7" s="6" t="s">
@@ -2406,1086 +2512,1086 @@
       <c r="F7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="20" t="s">
+      <c r="I7" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="20" t="s">
+      <c r="J7" s="22" t="s">
         <v>50</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="L7" s="20" t="s">
+      <c r="L7" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="M7" s="20" t="s">
+      <c r="M7" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="N7" s="20" t="s">
+      <c r="N7" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="O7" s="20" t="s">
+      <c r="O7" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="P7" s="18" t="s">
+      <c r="P7" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="Q7" s="26" t="s">
+      <c r="Q7" s="28" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="21" t="s">
+      <c r="F8" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="K8" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="L8" s="21" t="s">
+      <c r="L8" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="M8" s="21" t="s">
+      <c r="M8" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="N8" s="21" t="s">
+      <c r="N8" s="23" t="s">
         <v>63</v>
       </c>
       <c r="O8" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="P8" s="21" t="s">
+      <c r="P8" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="Q8" s="21" t="s">
+      <c r="Q8" s="23" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="9" s="7" customFormat="1" spans="1:17">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="23" t="s">
+      <c r="F9" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="H9" s="23" t="s">
+      <c r="H9" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="I9" s="23" t="s">
+      <c r="I9" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="23" t="s">
         <v>59</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="L9" s="21" t="s">
+      <c r="L9" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="M9" s="23" t="s">
+      <c r="M9" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="N9" s="23" t="s">
+      <c r="N9" s="25" t="s">
         <v>63</v>
       </c>
       <c r="O9" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="P9" s="23" t="s">
+      <c r="P9" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="Q9" s="23" t="s">
+      <c r="Q9" s="25" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="10" s="6" customFormat="1" spans="1:17">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="20" t="s">
+      <c r="F10" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="H10" s="22" t="s">
         <v>72</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="J10" s="20" t="s">
+      <c r="J10" s="22" t="s">
         <v>73</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="L10" s="20" t="s">
+      <c r="L10" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="M10" s="20" t="s">
+      <c r="M10" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="N10" s="20" t="s">
+      <c r="N10" s="22" t="s">
         <v>77</v>
       </c>
       <c r="O10" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="26" t="s">
+      <c r="P10" s="22"/>
+      <c r="Q10" s="28" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="11" s="6" customFormat="1" spans="1:17">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="20" t="s">
+      <c r="F11" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="H11" s="20" t="s">
+      <c r="H11" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="I11" s="20" t="s">
+      <c r="I11" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="J11" s="20" t="s">
+      <c r="J11" s="22" t="s">
         <v>83</v>
       </c>
       <c r="K11" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="L11" s="20" t="s">
+      <c r="L11" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="M11" s="20" t="s">
+      <c r="M11" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="N11" s="20" t="s">
+      <c r="N11" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="O11" s="20" t="s">
+      <c r="O11" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="P11" s="20" t="s">
+      <c r="P11" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="Q11" s="26" t="s">
+      <c r="Q11" s="28" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="12" s="6" customFormat="1" spans="1:17">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="20" t="s">
+      <c r="F12" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="H12" s="20" t="s">
+      <c r="H12" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="I12" s="20" t="s">
+      <c r="I12" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="J12" s="20" t="s">
+      <c r="J12" s="22" t="s">
         <v>88</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="L12" s="20" t="s">
+      <c r="L12" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="M12" s="20" t="s">
+      <c r="M12" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="N12" s="20" t="s">
+      <c r="N12" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="O12" s="20" t="s">
+      <c r="O12" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="P12" s="20" t="s">
+      <c r="P12" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="Q12" s="26" t="s">
+      <c r="Q12" s="28" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="13" s="6" customFormat="1" spans="1:17">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="20" t="s">
+      <c r="F13" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="H13" s="20" t="s">
+      <c r="H13" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="I13" s="20" t="s">
+      <c r="I13" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="J13" s="20" t="s">
+      <c r="J13" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="K13" s="20" t="s">
+      <c r="K13" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="L13" s="20" t="s">
+      <c r="L13" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="M13" s="20" t="s">
+      <c r="M13" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="N13" s="20" t="s">
+      <c r="N13" s="22" t="s">
         <v>94</v>
       </c>
       <c r="O13" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="P13" s="20" t="s">
+      <c r="P13" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="Q13" s="26" t="s">
+      <c r="Q13" s="28" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="14" s="6" customFormat="1" spans="1:17">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="20" t="s">
+      <c r="F14" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="H14" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="I14" s="20" t="s">
+      <c r="I14" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="J14" s="20" t="s">
+      <c r="J14" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="K14" s="20" t="s">
+      <c r="K14" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="L14" s="20" t="s">
+      <c r="L14" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="M14" s="20" t="s">
+      <c r="M14" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="N14" s="20" t="s">
+      <c r="N14" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="O14" s="20" t="s">
+      <c r="O14" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="P14" s="20" t="s">
+      <c r="P14" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="Q14" s="26" t="s">
+      <c r="Q14" s="28" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="15" s="6" customFormat="1" spans="1:17">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="20" t="s">
+      <c r="F15" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="I15" s="20" t="s">
+      <c r="I15" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="J15" s="20" t="s">
+      <c r="J15" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="K15" s="20" t="s">
+      <c r="K15" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="L15" s="20" t="s">
+      <c r="L15" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="M15" s="20" t="s">
+      <c r="M15" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="N15" s="20" t="s">
+      <c r="N15" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="O15" s="20" t="s">
+      <c r="O15" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="P15" s="20" t="s">
+      <c r="P15" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="Q15" s="26" t="s">
+      <c r="Q15" s="28" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="16" s="6" customFormat="1" spans="1:17">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="20" t="s">
+      <c r="F16" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="H16" s="20" t="s">
+      <c r="H16" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="I16" s="20" t="s">
+      <c r="I16" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="J16" s="20" t="s">
+      <c r="J16" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="K16" s="20" t="s">
+      <c r="K16" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="L16" s="20" t="s">
+      <c r="L16" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="M16" s="20" t="s">
+      <c r="M16" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="N16" s="20" t="s">
+      <c r="N16" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="O16" s="20" t="s">
+      <c r="O16" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="P16" s="20" t="s">
+      <c r="P16" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="Q16" s="26" t="s">
+      <c r="Q16" s="28" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="17" s="6" customFormat="1" spans="1:17">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="20" t="s">
+      <c r="F17" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="H17" s="20" t="s">
+      <c r="H17" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="I17" s="20" t="s">
+      <c r="I17" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="J17" s="20" t="s">
+      <c r="J17" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="K17" s="20" t="s">
+      <c r="K17" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="L17" s="20" t="s">
+      <c r="L17" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="M17" s="20" t="s">
+      <c r="M17" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="N17" s="20" t="s">
+      <c r="N17" s="22" t="s">
         <v>123</v>
       </c>
       <c r="O17" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="P17" s="20" t="s">
+      <c r="P17" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="Q17" s="26" t="s">
+      <c r="Q17" s="28" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="18" s="6" customFormat="1" spans="1:17">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" s="20" t="s">
+      <c r="F18" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="H18" s="20" t="s">
+      <c r="H18" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="I18" s="20" t="s">
+      <c r="I18" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="J18" s="20" t="s">
+      <c r="J18" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="K18" s="20" t="s">
+      <c r="K18" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="L18" s="20" t="s">
+      <c r="L18" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="M18" s="20" t="s">
+      <c r="M18" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="N18" s="20" t="s">
+      <c r="N18" s="22" t="s">
         <v>128</v>
       </c>
       <c r="O18" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="26" t="s">
+      <c r="P18" s="22"/>
+      <c r="Q18" s="28" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="19" s="6" customFormat="1" spans="1:17">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G19" s="20" t="s">
+      <c r="F19" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="H19" s="20" t="s">
+      <c r="H19" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="I19" s="20" t="s">
+      <c r="I19" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="J19" s="20" t="s">
+      <c r="J19" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="K19" s="20" t="s">
+      <c r="K19" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="L19" s="20" t="s">
+      <c r="L19" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="M19" s="20" t="s">
+      <c r="M19" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="N19" s="20" t="s">
+      <c r="N19" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="O19" s="20" t="s">
+      <c r="O19" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="26" t="s">
+      <c r="P19" s="22"/>
+      <c r="Q19" s="28" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="20" s="6" customFormat="1" spans="1:17">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20" s="20" t="s">
+      <c r="F20" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="H20" s="20" t="s">
+      <c r="H20" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="I20" s="20" t="s">
+      <c r="I20" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="J20" s="20" t="s">
+      <c r="J20" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="K20" s="20" t="s">
+      <c r="K20" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="L20" s="20" t="s">
+      <c r="L20" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="M20" s="20" t="s">
+      <c r="M20" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="N20" s="20" t="s">
+      <c r="N20" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="O20" s="20" t="s">
+      <c r="O20" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="26" t="s">
+      <c r="P20" s="22"/>
+      <c r="Q20" s="28" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="21" s="6" customFormat="1" spans="1:17">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F21" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" s="20" t="s">
+      <c r="F21" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="H21" s="20" t="s">
+      <c r="H21" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="I21" s="20" t="s">
+      <c r="I21" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="J21" s="20" t="s">
+      <c r="J21" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="K21" s="20" t="s">
+      <c r="K21" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="L21" s="20" t="s">
+      <c r="L21" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="M21" s="20" t="s">
+      <c r="M21" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="N21" s="20" t="s">
+      <c r="N21" s="22" t="s">
         <v>145</v>
       </c>
       <c r="O21" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="P21" s="20" t="s">
+      <c r="P21" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="Q21" s="26" t="s">
+      <c r="Q21" s="28" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="22" s="6" customFormat="1" spans="1:17">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F22" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G22" s="20" t="s">
+      <c r="F22" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="H22" s="20" t="s">
+      <c r="H22" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="I22" s="20" t="s">
+      <c r="I22" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="J22" s="20" t="s">
+      <c r="J22" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="K22" s="20" t="s">
+      <c r="K22" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="L22" s="20" t="s">
+      <c r="L22" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="M22" s="20" t="s">
+      <c r="M22" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="N22" s="20" t="s">
+      <c r="N22" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="O22" s="20" t="s">
+      <c r="O22" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="P22" s="20" t="s">
+      <c r="P22" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="Q22" s="26" t="s">
+      <c r="Q22" s="28" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="23" s="6" customFormat="1" spans="1:17">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E23" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F23" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="20" t="s">
+      <c r="F23" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="H23" s="20" t="s">
+      <c r="H23" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="I23" s="20" t="s">
+      <c r="I23" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="J23" s="20" t="s">
+      <c r="J23" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="K23" s="20" t="s">
+      <c r="K23" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="L23" s="20" t="s">
+      <c r="L23" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="M23" s="20" t="s">
+      <c r="M23" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="N23" s="20" t="s">
+      <c r="N23" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="O23" s="20" t="s">
+      <c r="O23" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="P23" s="20" t="s">
+      <c r="P23" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="Q23" s="26" t="s">
+      <c r="Q23" s="28" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="24" s="6" customFormat="1" spans="1:17">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D24" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="E24" s="20" t="s">
+      <c r="E24" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F24" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" s="20" t="s">
+      <c r="F24" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="H24" s="20" t="s">
+      <c r="H24" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="I24" s="20" t="s">
+      <c r="I24" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="J24" s="20" t="s">
+      <c r="J24" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="K24" s="20" t="s">
+      <c r="K24" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="L24" s="20" t="s">
+      <c r="L24" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="M24" s="20" t="s">
+      <c r="M24" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="N24" s="20" t="s">
+      <c r="N24" s="22" t="s">
         <v>152</v>
       </c>
-      <c r="O24" s="20" t="s">
+      <c r="O24" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="P24" s="20" t="s">
+      <c r="P24" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="Q24" s="26" t="s">
+      <c r="Q24" s="28" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="25" s="6" customFormat="1" spans="1:17">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="E25" s="20" t="s">
+      <c r="E25" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F25" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G25" s="20" t="s">
+      <c r="F25" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="H25" s="20" t="s">
+      <c r="H25" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="I25" s="20" t="s">
+      <c r="I25" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="J25" s="20" t="s">
+      <c r="J25" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="K25" s="20" t="s">
+      <c r="K25" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="L25" s="20" t="s">
+      <c r="L25" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="M25" s="20" t="s">
+      <c r="M25" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="N25" s="20" t="s">
+      <c r="N25" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="O25" s="20" t="s">
+      <c r="O25" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="P25" s="20" t="s">
+      <c r="P25" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="Q25" s="26" t="s">
+      <c r="Q25" s="28" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:17">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="D26" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="E26" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="F26" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" s="21" t="s">
+      <c r="F26" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="H26" s="21" t="s">
+      <c r="H26" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="I26" s="21" t="s">
+      <c r="I26" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="J26" s="21" t="s">
+      <c r="J26" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="K26" s="21" t="s">
+      <c r="K26" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="L26" s="21" t="s">
+      <c r="L26" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="M26" s="21" t="s">
+      <c r="M26" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="N26" s="21" t="s">
+      <c r="N26" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="O26" s="21" t="s">
+      <c r="O26" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="P26" s="21" t="s">
+      <c r="P26" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="Q26" s="20" t="s">
+      <c r="Q26" s="22" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="27" spans="1:17">
-      <c r="A27" s="21">
+      <c r="A27" s="23">
         <v>8086</v>
       </c>
-      <c r="B27" s="22">
+      <c r="B27" s="24">
         <v>1521</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="D27" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="E27" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="F27" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="G27" s="21" t="s">
+      <c r="F27" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="H27" s="21" t="s">
+      <c r="H27" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="I27" s="21" t="s">
+      <c r="I27" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="J27" s="21" t="s">
+      <c r="J27" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="K27" s="21" t="s">
+      <c r="K27" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="L27" s="21" t="s">
+      <c r="L27" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="M27" s="21" t="s">
+      <c r="M27" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="N27" s="21" t="s">
+      <c r="N27" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="O27" s="21" t="s">
+      <c r="O27" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="P27" s="21" t="s">
+      <c r="P27" s="23" t="s">
         <v>173</v>
       </c>
       <c r="Q27" s="6" t="s">
@@ -3493,758 +3599,758 @@
       </c>
     </row>
     <row r="28" s="6" customFormat="1" spans="1:17">
-      <c r="A28" s="20">
+      <c r="A28" s="22">
         <v>8086</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B28" s="20">
         <v>1572</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E28" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F28" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G28" s="20" t="s">
+      <c r="F28" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="H28" s="20" t="s">
+      <c r="H28" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="I28" s="20" t="s">
+      <c r="I28" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="J28" s="20" t="s">
+      <c r="J28" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="K28" s="20" t="s">
+      <c r="K28" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="L28" s="20" t="s">
+      <c r="L28" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="M28" s="20" t="s">
+      <c r="M28" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="N28" s="20" t="s">
+      <c r="N28" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="O28" s="20" t="s">
+      <c r="O28" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="P28" s="20" t="s">
+      <c r="P28" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="Q28" s="26" t="s">
+      <c r="Q28" s="28" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="29" s="6" customFormat="1" spans="1:17">
-      <c r="A29" s="20">
+      <c r="A29" s="22">
         <v>8086</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="20" t="s">
         <v>184</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="E29" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F29" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G29" s="20" t="s">
+      <c r="F29" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="H29" s="20" t="s">
+      <c r="H29" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="I29" s="20" t="s">
+      <c r="I29" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="J29" s="20" t="s">
+      <c r="J29" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="K29" s="20" t="s">
+      <c r="K29" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="L29" s="20" t="s">
+      <c r="L29" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="M29" s="20" t="s">
+      <c r="M29" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="N29" s="20" t="s">
+      <c r="N29" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="O29" s="20" t="s">
+      <c r="O29" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="P29" s="20" t="s">
+      <c r="P29" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="Q29" s="26" t="s">
+      <c r="Q29" s="28" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="30" s="6" customFormat="1" spans="1:17">
-      <c r="A30" s="20">
+      <c r="A30" s="22">
         <v>8086</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D30" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="E30" s="20" t="s">
+      <c r="E30" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F30" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G30" s="20" t="s">
+      <c r="F30" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="H30" s="20" t="s">
+      <c r="H30" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="I30" s="20" t="s">
+      <c r="I30" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="J30" s="20" t="s">
+      <c r="J30" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="K30" s="20" t="s">
+      <c r="K30" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="L30" s="20" t="s">
+      <c r="L30" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="M30" s="20" t="s">
+      <c r="M30" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="N30" s="20" t="s">
+      <c r="N30" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="O30" s="20" t="s">
+      <c r="O30" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="P30" s="20" t="s">
+      <c r="P30" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="Q30" s="26" t="s">
+      <c r="Q30" s="28" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="31" s="6" customFormat="1" spans="1:17">
-      <c r="A31" s="20">
+      <c r="A31" s="22">
         <v>8086</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="20" t="s">
+      <c r="D31" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="E31" s="20" t="s">
+      <c r="E31" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F31" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G31" s="20" t="s">
+      <c r="F31" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="H31" s="20" t="s">
+      <c r="H31" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="I31" s="20" t="s">
+      <c r="I31" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="J31" s="20" t="s">
+      <c r="J31" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="K31" s="20" t="s">
+      <c r="K31" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="L31" s="20" t="s">
+      <c r="L31" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="M31" s="20" t="s">
+      <c r="M31" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="N31" s="20" t="s">
+      <c r="N31" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="O31" s="20" t="s">
+      <c r="O31" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="P31" s="20" t="s">
+      <c r="P31" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="Q31" s="26" t="s">
+      <c r="Q31" s="28" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="32" s="6" customFormat="1" spans="1:17">
-      <c r="A32" s="20">
+      <c r="A32" s="22">
         <v>8086</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="20" t="s">
         <v>194</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D32" s="20" t="s">
+      <c r="D32" s="22" t="s">
         <v>195</v>
       </c>
-      <c r="E32" s="20" t="s">
+      <c r="E32" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F32" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G32" s="20" t="s">
+      <c r="F32" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G32" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="H32" s="20" t="s">
+      <c r="H32" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="I32" s="20" t="s">
+      <c r="I32" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="J32" s="20" t="s">
+      <c r="J32" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="K32" s="20" t="s">
+      <c r="K32" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="L32" s="20" t="s">
+      <c r="L32" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="M32" s="20" t="s">
+      <c r="M32" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="N32" s="20" t="s">
+      <c r="N32" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="O32" s="20" t="s">
+      <c r="O32" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="P32" s="20" t="s">
+      <c r="P32" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="Q32" s="26" t="s">
+      <c r="Q32" s="28" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="33" s="6" customFormat="1" spans="1:17">
-      <c r="A33" s="20">
+      <c r="A33" s="22">
         <v>8086</v>
       </c>
-      <c r="B33" s="18">
+      <c r="B33" s="20">
         <v>1572</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="20" t="s">
+      <c r="D33" s="22" t="s">
         <v>196</v>
       </c>
-      <c r="E33" s="20" t="s">
+      <c r="E33" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F33" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G33" s="20" t="s">
+      <c r="F33" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="H33" s="20" t="s">
+      <c r="H33" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="I33" s="20" t="s">
+      <c r="I33" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="J33" s="20" t="s">
+      <c r="J33" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="K33" s="20" t="s">
+      <c r="K33" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="L33" s="20" t="s">
+      <c r="L33" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="M33" s="20" t="s">
+      <c r="M33" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="N33" s="20" t="s">
+      <c r="N33" s="22" t="s">
         <v>198</v>
       </c>
-      <c r="O33" s="20" t="s">
+      <c r="O33" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="P33" s="20" t="s">
+      <c r="P33" s="22" t="s">
         <v>199</v>
       </c>
-      <c r="Q33" s="26" t="s">
+      <c r="Q33" s="28" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="34" s="6" customFormat="1" spans="1:17">
-      <c r="A34" s="20">
+      <c r="A34" s="22">
         <v>1000</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D34" s="20" t="s">
+      <c r="D34" s="22" t="s">
         <v>201</v>
       </c>
-      <c r="E34" s="20" t="s">
+      <c r="E34" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F34" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G34" s="20" t="s">
+      <c r="F34" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G34" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="H34" s="20" t="s">
+      <c r="H34" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="I34" s="20" t="s">
+      <c r="I34" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="J34" s="20" t="s">
+      <c r="J34" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="K34" s="20" t="s">
+      <c r="K34" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="L34" s="20" t="s">
+      <c r="L34" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="M34" s="20" t="s">
+      <c r="M34" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="N34" s="20" t="s">
+      <c r="N34" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="O34" s="20" t="s">
+      <c r="O34" s="22" t="s">
         <v>205</v>
       </c>
-      <c r="P34" s="20" t="s">
+      <c r="P34" s="22" t="s">
         <v>206</v>
       </c>
-      <c r="Q34" s="26" t="s">
+      <c r="Q34" s="28" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="35" s="6" customFormat="1" spans="1:17">
-      <c r="A35" s="20">
+      <c r="A35" s="22">
         <v>1000</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="D35" s="20">
+      <c r="D35" s="22">
         <v>9361</v>
       </c>
-      <c r="E35" s="20" t="s">
+      <c r="E35" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F35" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G35" s="20" t="s">
+      <c r="F35" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G35" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="H35" s="20" t="s">
+      <c r="H35" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="I35" s="20" t="s">
+      <c r="I35" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="J35" s="20" t="s">
+      <c r="J35" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="K35" s="20" t="s">
+      <c r="K35" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="L35" s="20" t="s">
+      <c r="L35" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="M35" s="20" t="s">
+      <c r="M35" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="N35" s="20" t="s">
+      <c r="N35" s="22" t="s">
         <v>209</v>
       </c>
-      <c r="O35" s="20" t="s">
+      <c r="O35" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="P35" s="20" t="s">
+      <c r="P35" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="Q35" s="26" t="s">
+      <c r="Q35" s="28" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="36" s="6" customFormat="1" spans="1:17">
-      <c r="A36" s="20">
+      <c r="A36" s="22">
         <v>1000</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C36" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D36" s="20" t="s">
+      <c r="D36" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="E36" s="20" t="s">
+      <c r="E36" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F36" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G36" s="20" t="s">
+      <c r="F36" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="H36" s="20" t="s">
+      <c r="H36" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="I36" s="20" t="s">
+      <c r="I36" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="J36" s="20" t="s">
+      <c r="J36" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="K36" s="20" t="s">
+      <c r="K36" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="L36" s="20" t="s">
+      <c r="L36" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="M36" s="20" t="s">
+      <c r="M36" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="N36" s="20" t="s">
+      <c r="N36" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="O36" s="20" t="s">
+      <c r="O36" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="P36" s="20" t="s">
+      <c r="P36" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="Q36" s="26" t="s">
+      <c r="Q36" s="28" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="37" s="6" customFormat="1" spans="1:17">
-      <c r="A37" s="20">
+      <c r="A37" s="22">
         <v>1000</v>
       </c>
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="C37" s="20" t="s">
+      <c r="C37" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D37" s="20" t="s">
+      <c r="D37" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="E37" s="20" t="s">
+      <c r="E37" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F37" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G37" s="20" t="s">
+      <c r="F37" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G37" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="H37" s="20" t="s">
+      <c r="H37" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="I37" s="20" t="s">
+      <c r="I37" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="J37" s="20" t="s">
+      <c r="J37" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="K37" s="20" t="s">
+      <c r="K37" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="L37" s="20" t="s">
+      <c r="L37" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="M37" s="20" t="s">
+      <c r="M37" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="N37" s="20" t="s">
+      <c r="N37" s="22" t="s">
         <v>215</v>
       </c>
-      <c r="O37" s="20" t="s">
+      <c r="O37" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="P37" s="20" t="s">
+      <c r="P37" s="22" t="s">
         <v>216</v>
       </c>
-      <c r="Q37" s="26" t="s">
+      <c r="Q37" s="28" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="38" s="6" customFormat="1" spans="1:17">
-      <c r="A38" s="20">
+      <c r="A38" s="22">
         <v>1000</v>
       </c>
-      <c r="B38" s="19" t="s">
+      <c r="B38" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="C38" s="20" t="s">
+      <c r="C38" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="D38" s="20">
+      <c r="D38" s="22">
         <v>9440</v>
       </c>
-      <c r="E38" s="20" t="s">
+      <c r="E38" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F38" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G38" s="20" t="s">
+      <c r="F38" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G38" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="H38" s="20" t="s">
+      <c r="H38" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="I38" s="20" t="s">
+      <c r="I38" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="J38" s="20" t="s">
+      <c r="J38" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="K38" s="20" t="s">
+      <c r="K38" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="L38" s="20" t="s">
+      <c r="L38" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="M38" s="20" t="s">
+      <c r="M38" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="N38" s="20" t="s">
+      <c r="N38" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="O38" s="20" t="s">
+      <c r="O38" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="P38" s="20" t="s">
+      <c r="P38" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="Q38" s="26" t="s">
+      <c r="Q38" s="28" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="39" s="6" customFormat="1" spans="1:17">
-      <c r="A39" s="20">
+      <c r="A39" s="22">
         <v>1000</v>
       </c>
-      <c r="B39" s="18" t="s">
+      <c r="B39" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="C39" s="20" t="s">
+      <c r="C39" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D39" s="20" t="s">
+      <c r="D39" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="E39" s="20" t="s">
+      <c r="E39" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F39" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G39" s="20" t="s">
+      <c r="F39" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="H39" s="20" t="s">
+      <c r="H39" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="I39" s="20" t="s">
+      <c r="I39" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="J39" s="20" t="s">
+      <c r="J39" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="K39" s="20" t="s">
+      <c r="K39" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="L39" s="20" t="s">
+      <c r="L39" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="M39" s="20" t="s">
+      <c r="M39" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="N39" s="20" t="s">
+      <c r="N39" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="O39" s="20" t="s">
+      <c r="O39" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="P39" s="20" t="s">
+      <c r="P39" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="Q39" s="26" t="s">
+      <c r="Q39" s="28" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="40" s="6" customFormat="1" spans="1:17">
-      <c r="A40" s="20">
+      <c r="A40" s="22">
         <v>1000</v>
       </c>
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="C40" s="20" t="s">
+      <c r="C40" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D40" s="20" t="s">
+      <c r="D40" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="E40" s="20" t="s">
+      <c r="E40" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F40" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G40" s="20" t="s">
+      <c r="F40" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G40" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="H40" s="20" t="s">
+      <c r="H40" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="I40" s="20" t="s">
+      <c r="I40" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="J40" s="20" t="s">
+      <c r="J40" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="K40" s="20" t="s">
+      <c r="K40" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="L40" s="20" t="s">
+      <c r="L40" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="M40" s="20" t="s">
+      <c r="M40" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="N40" s="20" t="s">
+      <c r="N40" s="22" t="s">
         <v>222</v>
       </c>
-      <c r="O40" s="20" t="s">
+      <c r="O40" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="P40" s="20" t="s">
+      <c r="P40" s="22" t="s">
         <v>223</v>
       </c>
-      <c r="Q40" s="26" t="s">
+      <c r="Q40" s="28" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="41" s="6" customFormat="1" spans="1:17">
-      <c r="A41" s="20">
+      <c r="A41" s="22">
         <v>1000</v>
       </c>
-      <c r="B41" s="18" t="s">
+      <c r="B41" s="20" t="s">
         <v>224</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C41" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D41" s="20" t="s">
+      <c r="D41" s="22" t="s">
         <v>225</v>
       </c>
-      <c r="E41" s="20" t="s">
+      <c r="E41" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F41" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G41" s="20" t="s">
+      <c r="F41" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G41" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="H41" s="20" t="s">
+      <c r="H41" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="I41" s="20" t="s">
+      <c r="I41" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="J41" s="20" t="s">
+      <c r="J41" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="K41" s="20" t="s">
+      <c r="K41" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="L41" s="20" t="s">
+      <c r="L41" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="M41" s="20" t="s">
+      <c r="M41" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="N41" s="20" t="s">
+      <c r="N41" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="O41" s="20" t="s">
+      <c r="O41" s="22" t="s">
         <v>227</v>
       </c>
-      <c r="P41" s="20" t="s">
+      <c r="P41" s="22" t="s">
         <v>228</v>
       </c>
-      <c r="Q41" s="26" t="s">
+      <c r="Q41" s="28" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="42" s="8" customFormat="1" spans="1:17">
-      <c r="A42" s="19">
+      <c r="A42" s="21">
         <v>1000</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="C42" s="19" t="s">
+      <c r="C42" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D42" s="18" t="s">
+      <c r="D42" s="20" t="s">
         <v>225</v>
       </c>
       <c r="E42" s="6" t="s">
@@ -4259,31 +4365,31 @@
       <c r="H42" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="I42" s="25" t="s">
+      <c r="I42" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="J42" s="20" t="s">
+      <c r="J42" s="22" t="s">
         <v>229</v>
       </c>
-      <c r="K42" s="20" t="s">
+      <c r="K42" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="L42" s="20" t="s">
+      <c r="L42" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="M42" s="25" t="s">
+      <c r="M42" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="N42" s="20" t="s">
+      <c r="N42" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="O42" s="20" t="s">
+      <c r="O42" s="22" t="s">
         <v>227</v>
       </c>
-      <c r="P42" s="18" t="s">
+      <c r="P42" s="20" t="s">
         <v>230</v>
       </c>
-      <c r="Q42" s="26" t="s">
+      <c r="Q42" s="28" t="s">
         <v>231</v>
       </c>
     </row>
@@ -4291,7 +4397,7 @@
       <c r="A43" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="B43" s="19" t="s">
+      <c r="B43" s="21" t="s">
         <v>233</v>
       </c>
       <c r="C43" s="6" t="s">
@@ -4309,83 +4415,83 @@
       <c r="G43" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="H43" s="20" t="s">
+      <c r="H43" s="22" t="s">
         <v>235</v>
       </c>
       <c r="I43" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J43" s="20" t="s">
+      <c r="J43" s="22" t="s">
         <v>236</v>
       </c>
       <c r="K43" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="L43" s="20" t="s">
+      <c r="L43" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="M43" s="20" t="s">
+      <c r="M43" s="22" t="s">
         <v>239</v>
       </c>
-      <c r="N43" s="20" t="s">
+      <c r="N43" s="22" t="s">
         <v>240</v>
       </c>
       <c r="O43" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="P43" s="18"/>
-      <c r="Q43" s="26" t="s">
+      <c r="P43" s="20"/>
+      <c r="Q43" s="28" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="44" s="9" customFormat="1" ht="14.45" customHeight="1" spans="1:17">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="22" t="s">
         <v>232</v>
       </c>
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="20" t="s">
         <v>233</v>
       </c>
-      <c r="C44" s="20" t="s">
+      <c r="C44" s="22" t="s">
         <v>232</v>
       </c>
-      <c r="D44" s="20" t="s">
+      <c r="D44" s="22" t="s">
         <v>243</v>
       </c>
-      <c r="E44" s="20" t="s">
+      <c r="E44" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F44" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G44" s="20" t="s">
+      <c r="F44" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G44" s="22" t="s">
         <v>234</v>
       </c>
-      <c r="H44" s="20" t="s">
+      <c r="H44" s="22" t="s">
         <v>235</v>
       </c>
-      <c r="I44" s="20" t="s">
+      <c r="I44" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="J44" s="20" t="s">
+      <c r="J44" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="K44" s="20" t="s">
+      <c r="K44" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="L44" s="20" t="s">
+      <c r="L44" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="M44" s="20" t="s">
+      <c r="M44" s="22" t="s">
         <v>239</v>
       </c>
-      <c r="N44" s="20" t="s">
+      <c r="N44" s="22" t="s">
         <v>240</v>
       </c>
       <c r="O44" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="P44" s="20"/>
-      <c r="Q44" s="26" t="s">
+      <c r="P44" s="22"/>
+      <c r="Q44" s="28" t="s">
         <v>242</v>
       </c>
     </row>
@@ -4393,7 +4499,7 @@
       <c r="A45" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="B45" s="19" t="s">
+      <c r="B45" s="21" t="s">
         <v>233</v>
       </c>
       <c r="C45" s="6" t="s">
@@ -4411,19 +4517,19 @@
       <c r="G45" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="H45" s="20" t="s">
+      <c r="H45" s="22" t="s">
         <v>235</v>
       </c>
-      <c r="I45" s="20" t="s">
+      <c r="I45" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="J45" s="20" t="s">
+      <c r="J45" s="22" t="s">
         <v>245</v>
       </c>
       <c r="K45" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="L45" s="20" t="s">
+      <c r="L45" s="22" t="s">
         <v>238</v>
       </c>
       <c r="M45" s="6" t="s">
@@ -4435,8 +4541,8 @@
       <c r="O45" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="P45" s="19"/>
-      <c r="Q45" s="26" t="s">
+      <c r="P45" s="21"/>
+      <c r="Q45" s="28" t="s">
         <v>242</v>
       </c>
     </row>
@@ -4444,7 +4550,7 @@
       <c r="A46" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="B46" s="21" t="s">
         <v>233</v>
       </c>
       <c r="C46" s="6" t="s">
@@ -4462,19 +4568,19 @@
       <c r="G46" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="H46" s="20" t="s">
+      <c r="H46" s="22" t="s">
         <v>235</v>
       </c>
-      <c r="I46" s="20" t="s">
+      <c r="I46" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="J46" s="20" t="s">
+      <c r="J46" s="22" t="s">
         <v>73</v>
       </c>
       <c r="K46" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="L46" s="20" t="s">
+      <c r="L46" s="22" t="s">
         <v>238</v>
       </c>
       <c r="M46" s="6" t="s">
@@ -4486,263 +4592,263 @@
       <c r="O46" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="P46" s="19"/>
-      <c r="Q46" s="26" t="s">
+      <c r="P46" s="21"/>
+      <c r="Q46" s="28" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="47" s="6" customFormat="1" spans="1:17">
-      <c r="A47" s="20">
+      <c r="A47" s="22">
         <v>1000</v>
       </c>
-      <c r="B47" s="18" t="s">
+      <c r="B47" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="C47" s="20" t="s">
+      <c r="C47" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D47" s="20" t="s">
+      <c r="D47" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="E47" s="20" t="s">
+      <c r="E47" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F47" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G47" s="20" t="s">
+      <c r="F47" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G47" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="H47" s="20" t="s">
+      <c r="H47" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="I47" s="20" t="s">
+      <c r="I47" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="J47" s="20" t="s">
+      <c r="J47" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="K47" s="20" t="s">
+      <c r="K47" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="L47" s="20" t="s">
+      <c r="L47" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="M47" s="20" t="s">
+      <c r="M47" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="N47" s="20" t="s">
+      <c r="N47" s="22" t="s">
         <v>249</v>
       </c>
-      <c r="O47" s="20" t="s">
+      <c r="O47" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="P47" s="20"/>
-      <c r="Q47" s="26" t="s">
+      <c r="P47" s="22"/>
+      <c r="Q47" s="28" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="48" s="6" customFormat="1" spans="1:17">
-      <c r="A48" s="20">
+      <c r="A48" s="22">
         <v>1000</v>
       </c>
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="C48" s="20" t="s">
+      <c r="C48" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D48" s="20" t="s">
+      <c r="D48" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="E48" s="20" t="s">
+      <c r="E48" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F48" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G48" s="20" t="s">
+      <c r="F48" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G48" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="H48" s="20" t="s">
+      <c r="H48" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="I48" s="20" t="s">
+      <c r="I48" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="J48" s="20" t="s">
+      <c r="J48" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="K48" s="20" t="s">
+      <c r="K48" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="L48" s="20" t="s">
+      <c r="L48" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="M48" s="20" t="s">
+      <c r="M48" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="N48" s="20" t="s">
+      <c r="N48" s="22" t="s">
         <v>250</v>
       </c>
-      <c r="O48" s="20" t="s">
+      <c r="O48" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="P48" s="20"/>
-      <c r="Q48" s="26" t="s">
+      <c r="P48" s="22"/>
+      <c r="Q48" s="28" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="49" s="6" customFormat="1" spans="1:17">
-      <c r="A49" s="20">
+      <c r="A49" s="22">
         <v>1000</v>
       </c>
-      <c r="B49" s="18" t="s">
+      <c r="B49" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="C49" s="20" t="s">
+      <c r="C49" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D49" s="20" t="s">
+      <c r="D49" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="E49" s="20" t="s">
+      <c r="E49" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F49" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G49" s="20" t="s">
+      <c r="F49" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G49" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="H49" s="20" t="s">
+      <c r="H49" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="I49" s="20" t="s">
+      <c r="I49" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="J49" s="20" t="s">
+      <c r="J49" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="K49" s="20" t="s">
+      <c r="K49" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="L49" s="20" t="s">
+      <c r="L49" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="M49" s="20" t="s">
+      <c r="M49" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="N49" s="20" t="s">
+      <c r="N49" s="22" t="s">
         <v>251</v>
       </c>
-      <c r="O49" s="20" t="s">
+      <c r="O49" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="P49" s="20"/>
-      <c r="Q49" s="26" t="s">
+      <c r="P49" s="22"/>
+      <c r="Q49" s="28" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="50" s="6" customFormat="1" spans="1:17">
-      <c r="A50" s="20">
+      <c r="A50" s="22">
         <v>1000</v>
       </c>
-      <c r="B50" s="18" t="s">
+      <c r="B50" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="C50" s="20" t="s">
+      <c r="C50" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D50" s="20" t="s">
+      <c r="D50" s="22" t="s">
         <v>252</v>
       </c>
-      <c r="E50" s="20" t="s">
+      <c r="E50" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F50" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G50" s="20" t="s">
+      <c r="F50" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G50" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="H50" s="20" t="s">
+      <c r="H50" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="I50" s="20" t="s">
+      <c r="I50" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="J50" s="20" t="s">
+      <c r="J50" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="K50" s="20" t="s">
+      <c r="K50" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="L50" s="20" t="s">
+      <c r="L50" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="M50" s="20" t="s">
+      <c r="M50" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="N50" s="20" t="s">
+      <c r="N50" s="22" t="s">
         <v>253</v>
       </c>
-      <c r="O50" s="20" t="s">
+      <c r="O50" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="P50" s="20"/>
-      <c r="Q50" s="26" t="s">
+      <c r="P50" s="22"/>
+      <c r="Q50" s="28" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="51" s="6" customFormat="1" spans="1:17">
-      <c r="A51" s="20">
+      <c r="A51" s="22">
         <v>1000</v>
       </c>
-      <c r="B51" s="18" t="s">
+      <c r="B51" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="C51" s="20" t="s">
+      <c r="C51" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D51" s="20" t="s">
+      <c r="D51" s="22" t="s">
         <v>254</v>
       </c>
-      <c r="E51" s="20" t="s">
+      <c r="E51" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F51" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G51" s="20" t="s">
+      <c r="F51" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G51" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="H51" s="20" t="s">
+      <c r="H51" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="I51" s="20" t="s">
+      <c r="I51" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="J51" s="20" t="s">
+      <c r="J51" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="K51" s="20" t="s">
+      <c r="K51" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="L51" s="20" t="s">
+      <c r="L51" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="M51" s="20" t="s">
+      <c r="M51" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="N51" s="20" t="s">
+      <c r="N51" s="22" t="s">
         <v>255</v>
       </c>
-      <c r="O51" s="20" t="s">
+      <c r="O51" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="P51" s="20"/>
-      <c r="Q51" s="26" t="s">
+      <c r="P51" s="22"/>
+      <c r="Q51" s="28" t="s">
         <v>207</v>
       </c>
     </row>
@@ -4750,10 +4856,10 @@
       <c r="A52" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="19" t="s">
+      <c r="B52" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="C52" s="20" t="s">
+      <c r="C52" s="22" t="s">
         <v>53</v>
       </c>
       <c r="D52" s="6" t="s">
@@ -4765,13 +4871,13 @@
       <c r="F52" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G52" s="20" t="s">
+      <c r="G52" s="22" t="s">
         <v>105</v>
       </c>
       <c r="H52" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="I52" s="20" t="s">
+      <c r="I52" s="22" t="s">
         <v>107</v>
       </c>
       <c r="J52" s="6" t="s">
@@ -4780,22 +4886,22 @@
       <c r="K52" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="L52" s="20" t="s">
+      <c r="L52" s="22" t="s">
         <v>260</v>
       </c>
-      <c r="M52" s="20" t="s">
+      <c r="M52" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="N52" s="20" t="s">
+      <c r="N52" s="22" t="s">
         <v>261</v>
       </c>
-      <c r="O52" s="20" t="s">
+      <c r="O52" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="P52" s="18" t="s">
+      <c r="P52" s="20" t="s">
         <v>263</v>
       </c>
-      <c r="Q52" s="26" t="s">
+      <c r="Q52" s="28" t="s">
         <v>264</v>
       </c>
     </row>
@@ -4803,10 +4909,10 @@
       <c r="A53" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B53" s="19" t="s">
+      <c r="B53" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="C53" s="20" t="s">
+      <c r="C53" s="22" t="s">
         <v>53</v>
       </c>
       <c r="D53" s="6" t="s">
@@ -4818,13 +4924,13 @@
       <c r="F53" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G53" s="20" t="s">
+      <c r="G53" s="22" t="s">
         <v>105</v>
       </c>
       <c r="H53" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="I53" s="20" t="s">
+      <c r="I53" s="22" t="s">
         <v>107</v>
       </c>
       <c r="J53" s="6" t="s">
@@ -4833,20 +4939,20 @@
       <c r="K53" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="L53" s="20" t="s">
+      <c r="L53" s="22" t="s">
         <v>260</v>
       </c>
-      <c r="M53" s="20" t="s">
+      <c r="M53" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="N53" s="20" t="s">
+      <c r="N53" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="O53" s="20" t="s">
+      <c r="O53" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="P53" s="18"/>
-      <c r="Q53" s="26" t="s">
+      <c r="P53" s="20"/>
+      <c r="Q53" s="28" t="s">
         <v>264</v>
       </c>
     </row>
@@ -4854,10 +4960,10 @@
       <c r="A54" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B54" s="19" t="s">
+      <c r="B54" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="C54" s="20" t="s">
+      <c r="C54" s="22" t="s">
         <v>53</v>
       </c>
       <c r="D54" s="6" t="s">
@@ -4869,13 +4975,13 @@
       <c r="F54" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G54" s="20" t="s">
+      <c r="G54" s="22" t="s">
         <v>105</v>
       </c>
       <c r="H54" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="I54" s="20" t="s">
+      <c r="I54" s="22" t="s">
         <v>107</v>
       </c>
       <c r="J54" s="6" t="s">
@@ -4884,34 +4990,34 @@
       <c r="K54" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="L54" s="20" t="s">
+      <c r="L54" s="22" t="s">
         <v>260</v>
       </c>
-      <c r="M54" s="20" t="s">
+      <c r="M54" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="N54" s="20" t="s">
+      <c r="N54" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="O54" s="20" t="s">
+      <c r="O54" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="P54" s="18"/>
-      <c r="Q54" s="26" t="s">
+      <c r="P54" s="20"/>
+      <c r="Q54" s="28" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="55" s="6" customFormat="1" spans="1:17">
-      <c r="A55" s="20" t="s">
+      <c r="A55" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B55" s="18" t="s">
+      <c r="B55" s="20" t="s">
         <v>267</v>
       </c>
-      <c r="C55" s="20" t="s">
+      <c r="C55" s="22" t="s">
         <v>268</v>
       </c>
-      <c r="D55" s="20" t="s">
+      <c r="D55" s="22" t="s">
         <v>269</v>
       </c>
       <c r="E55" s="6" t="s">
@@ -4920,13 +5026,13 @@
       <c r="F55" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G55" s="20" t="s">
+      <c r="G55" s="22" t="s">
         <v>270</v>
       </c>
-      <c r="I55" s="20" t="s">
+      <c r="I55" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="J55" s="20" t="s">
+      <c r="J55" s="22" t="s">
         <v>272</v>
       </c>
       <c r="K55" s="6" t="s">
@@ -4935,46 +5041,46 @@
       <c r="L55" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="M55" s="20" t="s">
+      <c r="M55" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="N55" s="20" t="s">
+      <c r="N55" s="22" t="s">
         <v>275</v>
       </c>
-      <c r="O55" s="20" t="s">
+      <c r="O55" s="22" t="s">
         <v>275</v>
       </c>
-      <c r="P55" s="19"/>
-      <c r="Q55" s="26" t="s">
+      <c r="P55" s="21"/>
+      <c r="Q55" s="28" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="56" s="6" customFormat="1" spans="1:17">
-      <c r="A56" s="20" t="s">
+      <c r="A56" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B56" s="18" t="s">
+      <c r="B56" s="20" t="s">
         <v>267</v>
       </c>
-      <c r="C56" s="20" t="s">
+      <c r="C56" s="22" t="s">
         <v>268</v>
       </c>
-      <c r="D56" s="20" t="s">
+      <c r="D56" s="22" t="s">
         <v>269</v>
       </c>
-      <c r="E56" s="20" t="s">
+      <c r="E56" s="22" t="s">
         <v>141</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G56" s="20" t="s">
+      <c r="G56" s="22" t="s">
         <v>270</v>
       </c>
-      <c r="I56" s="20" t="s">
+      <c r="I56" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="J56" s="20" t="s">
+      <c r="J56" s="22" t="s">
         <v>272</v>
       </c>
       <c r="K56" s="6" t="s">
@@ -4983,31 +5089,31 @@
       <c r="L56" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="M56" s="20" t="s">
+      <c r="M56" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="N56" s="20" t="s">
+      <c r="N56" s="22" t="s">
         <v>275</v>
       </c>
-      <c r="O56" s="20" t="s">
+      <c r="O56" s="22" t="s">
         <v>275</v>
       </c>
-      <c r="P56" s="19"/>
-      <c r="Q56" s="26" t="s">
+      <c r="P56" s="21"/>
+      <c r="Q56" s="28" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="57" s="6" customFormat="1" spans="1:17">
-      <c r="A57" s="20" t="s">
+      <c r="A57" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B57" s="18" t="s">
+      <c r="B57" s="20" t="s">
         <v>277</v>
       </c>
-      <c r="C57" s="20" t="s">
+      <c r="C57" s="22" t="s">
         <v>268</v>
       </c>
-      <c r="D57" s="20" t="s">
+      <c r="D57" s="22" t="s">
         <v>269</v>
       </c>
       <c r="E57" s="6" t="s">
@@ -5016,13 +5122,13 @@
       <c r="F57" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G57" s="20" t="s">
+      <c r="G57" s="22" t="s">
         <v>270</v>
       </c>
-      <c r="I57" s="20" t="s">
+      <c r="I57" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="J57" s="20" t="s">
+      <c r="J57" s="22" t="s">
         <v>272</v>
       </c>
       <c r="K57" s="6" t="s">
@@ -5031,46 +5137,46 @@
       <c r="L57" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="M57" s="20" t="s">
+      <c r="M57" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="N57" s="20" t="s">
+      <c r="N57" s="22" t="s">
         <v>279</v>
       </c>
-      <c r="O57" s="20" t="s">
+      <c r="O57" s="22" t="s">
         <v>279</v>
       </c>
-      <c r="P57" s="19"/>
-      <c r="Q57" s="26" t="s">
+      <c r="P57" s="21"/>
+      <c r="Q57" s="28" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="58" s="6" customFormat="1" spans="1:17">
-      <c r="A58" s="20" t="s">
+      <c r="A58" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B58" s="18" t="s">
+      <c r="B58" s="20" t="s">
         <v>277</v>
       </c>
-      <c r="C58" s="20" t="s">
+      <c r="C58" s="22" t="s">
         <v>268</v>
       </c>
-      <c r="D58" s="20" t="s">
+      <c r="D58" s="22" t="s">
         <v>269</v>
       </c>
-      <c r="E58" s="20" t="s">
+      <c r="E58" s="22" t="s">
         <v>141</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G58" s="20" t="s">
+      <c r="G58" s="22" t="s">
         <v>270</v>
       </c>
-      <c r="I58" s="20" t="s">
+      <c r="I58" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="J58" s="20" t="s">
+      <c r="J58" s="22" t="s">
         <v>272</v>
       </c>
       <c r="K58" s="6" t="s">
@@ -5079,31 +5185,31 @@
       <c r="L58" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="M58" s="20" t="s">
+      <c r="M58" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="N58" s="20" t="s">
+      <c r="N58" s="22" t="s">
         <v>279</v>
       </c>
-      <c r="O58" s="20" t="s">
+      <c r="O58" s="22" t="s">
         <v>279</v>
       </c>
-      <c r="P58" s="19"/>
-      <c r="Q58" s="26" t="s">
+      <c r="P58" s="21"/>
+      <c r="Q58" s="28" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="59" s="6" customFormat="1" spans="1:17">
-      <c r="A59" s="20" t="s">
+      <c r="A59" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B59" s="18" t="s">
+      <c r="B59" s="20" t="s">
         <v>281</v>
       </c>
-      <c r="C59" s="20" t="s">
+      <c r="C59" s="22" t="s">
         <v>268</v>
       </c>
-      <c r="D59" s="20" t="s">
+      <c r="D59" s="22" t="s">
         <v>269</v>
       </c>
       <c r="E59" s="6" t="s">
@@ -5112,13 +5218,13 @@
       <c r="F59" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G59" s="20" t="s">
+      <c r="G59" s="22" t="s">
         <v>270</v>
       </c>
-      <c r="I59" s="20" t="s">
+      <c r="I59" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="J59" s="20" t="s">
+      <c r="J59" s="22" t="s">
         <v>272</v>
       </c>
       <c r="K59" s="6" t="s">
@@ -5127,48 +5233,48 @@
       <c r="L59" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="M59" s="20" t="s">
+      <c r="M59" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="N59" s="20" t="s">
+      <c r="N59" s="22" t="s">
         <v>283</v>
       </c>
-      <c r="O59" s="20" t="s">
+      <c r="O59" s="22" t="s">
         <v>283</v>
       </c>
-      <c r="P59" s="18" t="s">
+      <c r="P59" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="Q59" s="26" t="s">
+      <c r="Q59" s="28" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="60" s="6" customFormat="1" spans="1:17">
-      <c r="A60" s="20" t="s">
+      <c r="A60" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B60" s="18" t="s">
+      <c r="B60" s="20" t="s">
         <v>281</v>
       </c>
-      <c r="C60" s="20" t="s">
+      <c r="C60" s="22" t="s">
         <v>268</v>
       </c>
-      <c r="D60" s="20" t="s">
+      <c r="D60" s="22" t="s">
         <v>269</v>
       </c>
-      <c r="E60" s="20" t="s">
+      <c r="E60" s="22" t="s">
         <v>141</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G60" s="20" t="s">
+      <c r="G60" s="22" t="s">
         <v>270</v>
       </c>
-      <c r="I60" s="20" t="s">
+      <c r="I60" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="J60" s="20" t="s">
+      <c r="J60" s="22" t="s">
         <v>272</v>
       </c>
       <c r="K60" s="6" t="s">
@@ -5177,33 +5283,33 @@
       <c r="L60" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="M60" s="20" t="s">
+      <c r="M60" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="N60" s="20" t="s">
+      <c r="N60" s="22" t="s">
         <v>283</v>
       </c>
-      <c r="O60" s="20" t="s">
+      <c r="O60" s="22" t="s">
         <v>283</v>
       </c>
-      <c r="P60" s="18" t="s">
+      <c r="P60" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="Q60" s="26" t="s">
+      <c r="Q60" s="28" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="61" s="6" customFormat="1" spans="1:17">
-      <c r="A61" s="20" t="s">
+      <c r="A61" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B61" s="18" t="s">
+      <c r="B61" s="20" t="s">
         <v>281</v>
       </c>
-      <c r="C61" s="20" t="s">
+      <c r="C61" s="22" t="s">
         <v>268</v>
       </c>
-      <c r="D61" s="20" t="s">
+      <c r="D61" s="22" t="s">
         <v>269</v>
       </c>
       <c r="E61" s="6" t="s">
@@ -5212,13 +5318,13 @@
       <c r="F61" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G61" s="20" t="s">
+      <c r="G61" s="22" t="s">
         <v>270</v>
       </c>
-      <c r="I61" s="20" t="s">
+      <c r="I61" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="J61" s="20" t="s">
+      <c r="J61" s="22" t="s">
         <v>272</v>
       </c>
       <c r="K61" s="6" t="s">
@@ -5227,48 +5333,48 @@
       <c r="L61" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="M61" s="20" t="s">
+      <c r="M61" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="N61" s="20" t="s">
+      <c r="N61" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="O61" s="20" t="s">
+      <c r="O61" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="P61" s="18" t="s">
+      <c r="P61" s="20" t="s">
         <v>287</v>
       </c>
-      <c r="Q61" s="26" t="s">
+      <c r="Q61" s="28" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="62" s="6" customFormat="1" spans="1:17">
-      <c r="A62" s="20" t="s">
+      <c r="A62" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B62" s="18" t="s">
+      <c r="B62" s="20" t="s">
         <v>281</v>
       </c>
-      <c r="C62" s="20" t="s">
+      <c r="C62" s="22" t="s">
         <v>268</v>
       </c>
-      <c r="D62" s="20" t="s">
+      <c r="D62" s="22" t="s">
         <v>269</v>
       </c>
-      <c r="E62" s="20" t="s">
+      <c r="E62" s="22" t="s">
         <v>141</v>
       </c>
       <c r="F62" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G62" s="20" t="s">
+      <c r="G62" s="22" t="s">
         <v>270</v>
       </c>
-      <c r="I62" s="20" t="s">
+      <c r="I62" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="J62" s="20" t="s">
+      <c r="J62" s="22" t="s">
         <v>272</v>
       </c>
       <c r="K62" s="6" t="s">
@@ -5277,32 +5383,522 @@
       <c r="L62" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="M62" s="20" t="s">
+      <c r="M62" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="N62" s="20" t="s">
+      <c r="N62" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="O62" s="20" t="s">
+      <c r="O62" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="P62" s="18" t="s">
+      <c r="P62" s="20" t="s">
         <v>287</v>
       </c>
-      <c r="Q62" s="26" t="s">
+      <c r="Q62" s="28" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="63" s="6" customFormat="1" spans="2:16">
-      <c r="B63" s="19"/>
-      <c r="P63" s="19"/>
-    </row>
-    <row r="64" s="6" customFormat="1" spans="2:16">
-      <c r="B64" s="19"/>
-      <c r="P64" s="19"/>
+    <row r="63" s="10" customFormat="1" spans="1:17">
+      <c r="A63" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G63" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H63" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="I63" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J63" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="K63" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="L63" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="M63" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="N63" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="O63" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="P63" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="Q63" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="64" s="10" customFormat="1" spans="1:17">
+      <c r="A64" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F64" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G64" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="H64" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="I64" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J64" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="K64" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="L64" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="M64" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="N64" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="O64" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="P64" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="Q64" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" s="10" customFormat="1" spans="1:17">
+      <c r="A65" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G65" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H65" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="I65" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="J65" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="K65" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="L65" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="M65" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="N65" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="O65" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="P65" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q65" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" s="10" customFormat="1" spans="1:17">
+      <c r="A66" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F66" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G66" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="H66" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="I66" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J66" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="K66" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="L66" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="M66" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="N66" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="O66" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="P66" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="Q66" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" s="10" customFormat="1" spans="1:17">
+      <c r="A67" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F67" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G67" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H67" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="I67" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J67" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="K67" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="L67" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="M67" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="N67" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="O67" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="P67" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q67" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="68" s="10" customFormat="1" spans="1:17">
+      <c r="A68" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="E68" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F68" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G68" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H68" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="I68" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J68" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="K68" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="L68" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="M68" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="N68" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="O68" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="P68" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q68" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="69" s="10" customFormat="1" spans="1:17">
+      <c r="A69" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E69" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F69" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G69" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H69" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="I69" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J69" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="K69" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="L69" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="M69" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="N69" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="O69" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="P69" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="Q69" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="70" s="10" customFormat="1" spans="1:17">
+      <c r="A70" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E70" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F70" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G70" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H70" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="I70" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J70" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="K70" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="L70" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="M70" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="N70" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="O70" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="P70" s="10"/>
+      <c r="Q70" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" s="10" customFormat="1" spans="1:17">
+      <c r="A71" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F71" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G71" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="H71" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="I71" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J71" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="K71" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="L71" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="M71" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="N71" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="O71" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="P71" s="10"/>
+      <c r="Q71" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="72" s="11" customFormat="1"/>
+    <row r="73" s="11" customFormat="1"/>
+    <row r="74" s="11" customFormat="1"/>
+    <row r="75" s="11" customFormat="1"/>
+    <row r="76" s="11" customFormat="1"/>
+    <row r="77" s="11" customFormat="1"/>
+    <row r="78" s="11" customFormat="1"/>
+    <row r="79" s="11" customFormat="1"/>
+    <row r="80" s="11" customFormat="1"/>
+    <row r="81" s="11" customFormat="1"/>
+    <row r="82" s="11" customFormat="1"/>
+    <row r="83" s="11" customFormat="1"/>
+    <row r="84" s="11" customFormat="1"/>
+    <row r="85" s="11" customFormat="1"/>
+    <row r="86" s="11" customFormat="1"/>
+    <row r="87" s="11" customFormat="1"/>
+    <row r="88" s="11" customFormat="1"/>
+    <row r="89" s="11" customFormat="1"/>
+    <row r="90" s="11" customFormat="1"/>
+    <row r="91" s="11" customFormat="1"/>
+    <row r="92" s="11" customFormat="1"/>
+    <row r="93" s="12" customFormat="1" spans="2:16">
+      <c r="B93" s="13"/>
+      <c r="P93" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q62">
+  <autoFilter ref="A1:Q92">
     <extLst/>
   </autoFilter>
   <hyperlinks>

</xml_diff>